<commit_message>
tried to run code and update risk
</commit_message>
<xml_diff>
--- a/data/cumulative_ma_data.xlsx
+++ b/data/cumulative_ma_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/de77e8898af74b83/Documents/Risk MetaAnalysis Rui/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rmata/Documents/GitHub/cumulative/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="879" documentId="13_ncr:1_{C2B7AADA-945F-470F-8BD4-634B2EC360CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1A90B065-99D7-4335-9525-0ED3A2E7E4BD}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35077E81-9049-0946-AA62-D1EC3E32E4A3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" activeTab="3" xr2:uid="{D15F3EFF-771D-497D-BAA4-C31EA9079474}"/>
+    <workbookView xWindow="13640" yWindow="600" windowWidth="34720" windowHeight="21340" xr2:uid="{D15F3EFF-771D-497D-BAA4-C31EA9079474}"/>
   </bookViews>
   <sheets>
     <sheet name="Mata_et_al(2011)" sheetId="2" r:id="rId1"/>
@@ -22,15 +22,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -623,7 +614,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -654,6 +645,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -970,16 +962,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38FBD286-E9F4-43DE-AE76-F152A62FC2EB}">
   <dimension ref="A1:R46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P23" sqref="P23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17:F32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.06640625" style="1"/>
+    <col min="1" max="1" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>42</v>
       </c>
@@ -1020,7 +1012,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -1035,6 +1027,10 @@
       </c>
       <c r="E2" s="5">
         <v>16</v>
+      </c>
+      <c r="F2" s="16">
+        <f>D2+E2</f>
+        <v>32</v>
       </c>
       <c r="G2" s="4">
         <v>25</v>
@@ -1062,7 +1058,7 @@
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -1077,6 +1073,10 @@
       </c>
       <c r="E3" s="5">
         <v>39</v>
+      </c>
+      <c r="F3" s="16">
+        <f t="shared" ref="F3:F9" si="0">D3+E3</f>
+        <v>78</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>76</v>
@@ -1105,7 +1105,7 @@
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1121,6 +1121,10 @@
       <c r="E4" s="5">
         <v>56</v>
       </c>
+      <c r="F4" s="16">
+        <f t="shared" si="0"/>
+        <v>119</v>
+      </c>
       <c r="G4" s="4">
         <v>24.9</v>
       </c>
@@ -1145,7 +1149,7 @@
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>49</v>
       </c>
@@ -1160,6 +1164,10 @@
       </c>
       <c r="E5" s="5">
         <v>45</v>
+      </c>
+      <c r="F5" s="16">
+        <f t="shared" si="0"/>
+        <v>86</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>77</v>
@@ -1187,7 +1195,7 @@
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>50</v>
       </c>
@@ -1202,6 +1210,10 @@
       </c>
       <c r="E6" s="5">
         <v>40</v>
+      </c>
+      <c r="F6" s="16">
+        <f t="shared" si="0"/>
+        <v>80</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>78</v>
@@ -1230,7 +1242,7 @@
       <c r="Q6" s="2"/>
       <c r="R6" s="2"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>50</v>
       </c>
@@ -1245,6 +1257,10 @@
       </c>
       <c r="E7" s="5">
         <v>79</v>
+      </c>
+      <c r="F7" s="16">
+        <f t="shared" si="0"/>
+        <v>152</v>
       </c>
       <c r="G7" s="4">
         <v>74</v>
@@ -1273,7 +1289,7 @@
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>51</v>
       </c>
@@ -1288,6 +1304,10 @@
       </c>
       <c r="E8" s="5">
         <v>18</v>
+      </c>
+      <c r="F8" s="16">
+        <f t="shared" si="0"/>
+        <v>36</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>79</v>
@@ -1315,7 +1335,7 @@
       <c r="Q8" s="2"/>
       <c r="R8" s="2"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>52</v>
       </c>
@@ -1330,6 +1350,10 @@
       </c>
       <c r="E9" s="5">
         <v>52</v>
+      </c>
+      <c r="F9" s="16">
+        <f t="shared" si="0"/>
+        <v>164</v>
       </c>
       <c r="G9" s="4">
         <v>37.799999999999997</v>
@@ -1358,7 +1382,7 @@
       <c r="Q9" s="2"/>
       <c r="R9" s="2"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>53</v>
       </c>
@@ -1403,7 +1427,7 @@
       <c r="Q10" s="2"/>
       <c r="R10" s="2"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>53</v>
       </c>
@@ -1446,7 +1470,7 @@
       <c r="O11" s="2"/>
       <c r="P11" s="2"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>53</v>
       </c>
@@ -1492,7 +1516,7 @@
       <c r="Q12" s="2"/>
       <c r="R12" s="2"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -1507,6 +1531,10 @@
       </c>
       <c r="E13" s="5">
         <v>24</v>
+      </c>
+      <c r="F13" s="16">
+        <f t="shared" ref="F13:F14" si="1">D13+E13</f>
+        <v>48</v>
       </c>
       <c r="G13" s="4">
         <v>24.2</v>
@@ -1535,7 +1563,7 @@
       <c r="Q13" s="11"/>
       <c r="R13" s="11"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>54</v>
       </c>
@@ -1551,6 +1579,10 @@
       <c r="E14" s="5">
         <v>40</v>
       </c>
+      <c r="F14" s="16">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
       <c r="G14" s="4">
         <v>27.9</v>
       </c>
@@ -1573,7 +1605,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>55</v>
       </c>
@@ -1614,7 +1646,7 @@
         <v>1.35</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>55</v>
       </c>
@@ -1660,7 +1692,7 @@
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>56</v>
       </c>
@@ -1676,6 +1708,10 @@
       <c r="E17" s="5">
         <v>20</v>
       </c>
+      <c r="F17" s="16">
+        <f t="shared" ref="F17:F32" si="2">D17+E17</f>
+        <v>43</v>
+      </c>
       <c r="G17" s="4">
         <v>28.4</v>
       </c>
@@ -1700,7 +1736,7 @@
       <c r="O17" s="2"/>
       <c r="P17" s="2"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>57</v>
       </c>
@@ -1715,6 +1751,10 @@
       </c>
       <c r="E18" s="5">
         <v>23</v>
+      </c>
+      <c r="F18" s="16">
+        <f t="shared" si="2"/>
+        <v>49</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>80</v>
@@ -1742,7 +1782,7 @@
       <c r="Q18" s="2"/>
       <c r="R18" s="2"/>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>58</v>
       </c>
@@ -1757,6 +1797,10 @@
       </c>
       <c r="E19" s="5">
         <v>9</v>
+      </c>
+      <c r="F19" s="16">
+        <f t="shared" si="2"/>
+        <v>21</v>
       </c>
       <c r="G19" s="4">
         <v>29.2</v>
@@ -1785,7 +1829,7 @@
       <c r="Q19" s="2"/>
       <c r="R19" s="2"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>59</v>
       </c>
@@ -1801,6 +1845,10 @@
       <c r="E20" s="5">
         <v>30</v>
       </c>
+      <c r="F20" s="16">
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
       <c r="G20" s="4">
         <v>28.8</v>
       </c>
@@ -1825,7 +1873,7 @@
       <c r="O20" s="2"/>
       <c r="P20" s="2"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>17</v>
       </c>
@@ -1841,6 +1889,10 @@
       <c r="E21" s="5">
         <v>58</v>
       </c>
+      <c r="F21" s="16">
+        <f t="shared" si="2"/>
+        <v>116</v>
+      </c>
       <c r="G21" s="4">
         <v>20.3</v>
       </c>
@@ -1865,7 +1917,7 @@
       <c r="O21" s="2"/>
       <c r="P21" s="2"/>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -1880,6 +1932,10 @@
       </c>
       <c r="E22" s="5">
         <v>22</v>
+      </c>
+      <c r="F22" s="16">
+        <f t="shared" si="2"/>
+        <v>44</v>
       </c>
       <c r="G22" s="4">
         <v>19.8</v>
@@ -1907,7 +1963,7 @@
       <c r="Q22" s="2"/>
       <c r="R22" s="2"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>60</v>
       </c>
@@ -1922,6 +1978,10 @@
       </c>
       <c r="E23" s="5">
         <v>45</v>
+      </c>
+      <c r="F23" s="16">
+        <f t="shared" si="2"/>
+        <v>87</v>
       </c>
       <c r="G23" s="4">
         <v>20.9</v>
@@ -1949,7 +2009,7 @@
       <c r="Q23" s="2"/>
       <c r="R23" s="2"/>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>61</v>
       </c>
@@ -1964,6 +2024,10 @@
       </c>
       <c r="E24" s="5">
         <v>53</v>
+      </c>
+      <c r="F24" s="16">
+        <f t="shared" si="2"/>
+        <v>103</v>
       </c>
       <c r="G24" s="4">
         <v>21</v>
@@ -1992,7 +2056,7 @@
       <c r="Q24" s="2"/>
       <c r="R24" s="2"/>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>62</v>
       </c>
@@ -2008,6 +2072,10 @@
       <c r="E25" s="5">
         <v>44</v>
       </c>
+      <c r="F25" s="16">
+        <f t="shared" si="2"/>
+        <v>84</v>
+      </c>
       <c r="G25" s="4">
         <v>19.3</v>
       </c>
@@ -2032,7 +2100,7 @@
       <c r="O25" s="2"/>
       <c r="P25" s="2"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>87</v>
       </c>
@@ -2047,6 +2115,10 @@
       </c>
       <c r="E26" s="5">
         <v>192</v>
+      </c>
+      <c r="F26" s="16">
+        <f t="shared" si="2"/>
+        <v>384</v>
       </c>
       <c r="G26" s="4">
         <v>23.9</v>
@@ -2075,7 +2147,7 @@
       <c r="Q26" s="2"/>
       <c r="R26" s="2"/>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>63</v>
       </c>
@@ -2090,6 +2162,10 @@
       </c>
       <c r="E27" s="5">
         <v>42</v>
+      </c>
+      <c r="F27" s="16">
+        <f t="shared" si="2"/>
+        <v>77</v>
       </c>
       <c r="G27" s="4">
         <v>25.7</v>
@@ -2118,7 +2194,7 @@
       <c r="Q27" s="2"/>
       <c r="R27" s="2"/>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>63</v>
       </c>
@@ -2133,6 +2209,10 @@
       </c>
       <c r="E28" s="5">
         <v>59</v>
+      </c>
+      <c r="F28" s="16">
+        <f t="shared" si="2"/>
+        <v>108</v>
       </c>
       <c r="G28" s="4">
         <v>27.3</v>
@@ -2159,7 +2239,7 @@
       <c r="O28" s="2"/>
       <c r="P28" s="2"/>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>22</v>
       </c>
@@ -2174,6 +2254,10 @@
       </c>
       <c r="E29" s="5">
         <v>24</v>
+      </c>
+      <c r="F29" s="16">
+        <f t="shared" si="2"/>
+        <v>75</v>
       </c>
       <c r="G29" s="4">
         <v>25</v>
@@ -2200,7 +2284,7 @@
       <c r="O29" s="2"/>
       <c r="P29" s="2"/>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>64</v>
       </c>
@@ -2216,6 +2300,10 @@
       <c r="E30" s="5">
         <v>168</v>
       </c>
+      <c r="F30" s="16">
+        <f t="shared" si="2"/>
+        <v>829</v>
+      </c>
       <c r="G30" s="4">
         <v>44.8</v>
       </c>
@@ -2240,7 +2328,7 @@
       <c r="O30" s="2"/>
       <c r="P30" s="2"/>
     </row>
-    <row r="31" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>65</v>
       </c>
@@ -2256,7 +2344,10 @@
       <c r="E31" s="5">
         <v>61</v>
       </c>
-      <c r="F31"/>
+      <c r="F31" s="16">
+        <f t="shared" si="2"/>
+        <v>419</v>
+      </c>
       <c r="G31" s="4" t="s">
         <v>79</v>
       </c>
@@ -2284,7 +2375,7 @@
       <c r="Q31" s="2"/>
       <c r="R31" s="2"/>
     </row>
-    <row r="32" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>66</v>
       </c>
@@ -2300,7 +2391,10 @@
       <c r="E32" s="5">
         <v>63</v>
       </c>
-      <c r="F32"/>
+      <c r="F32" s="16">
+        <f t="shared" si="2"/>
+        <v>150</v>
+      </c>
       <c r="G32" s="4">
         <v>23</v>
       </c>
@@ -2327,7 +2421,7 @@
       <c r="Q32" s="2"/>
       <c r="R32" s="2"/>
     </row>
-    <row r="33" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>67</v>
       </c>
@@ -2368,7 +2462,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="34" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>67</v>
       </c>
@@ -2410,10 +2504,10 @@
       </c>
       <c r="O34" s="9"/>
     </row>
-    <row r="35" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="36" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="37" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="38" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="13"/>
       <c r="B38" s="13"/>
       <c r="C38" s="13"/>
@@ -2428,7 +2522,7 @@
       <c r="L38" s="13"/>
       <c r="M38" s="13"/>
     </row>
-    <row r="39" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="13"/>
       <c r="B39" s="13"/>
       <c r="C39" s="13"/>
@@ -2443,7 +2537,7 @@
       <c r="L39" s="13"/>
       <c r="M39" s="13"/>
     </row>
-    <row r="40" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="13"/>
       <c r="B40" s="13"/>
       <c r="C40" s="13"/>
@@ -2458,7 +2552,7 @@
       <c r="L40" s="13"/>
       <c r="M40" s="13"/>
     </row>
-    <row r="41" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="13"/>
       <c r="B41" s="13"/>
       <c r="C41" s="13"/>
@@ -2473,7 +2567,7 @@
       <c r="L41" s="13"/>
       <c r="M41" s="13"/>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A42" s="13"/>
       <c r="B42" s="13"/>
       <c r="C42" s="13"/>
@@ -2488,7 +2582,7 @@
       <c r="L42" s="13"/>
       <c r="M42" s="13"/>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A43" s="13"/>
       <c r="B43" s="13"/>
       <c r="C43" s="13"/>
@@ -2503,7 +2597,7 @@
       <c r="L43" s="13"/>
       <c r="M43" s="13"/>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A44" s="13"/>
       <c r="B44" s="13"/>
       <c r="C44" s="13"/>
@@ -2518,7 +2612,7 @@
       <c r="L44" s="13"/>
       <c r="M44" s="13"/>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A45" s="13"/>
       <c r="B45" s="13"/>
       <c r="C45" s="13"/>
@@ -2533,7 +2627,7 @@
       <c r="L45" s="13"/>
       <c r="M45" s="13"/>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A46" s="13"/>
       <c r="B46" s="13"/>
       <c r="C46" s="13"/>
@@ -2563,9 +2657,9 @@
       <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>42</v>
       </c>
@@ -2591,7 +2685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -2617,7 +2711,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -2643,7 +2737,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -2669,7 +2763,7 @@
         <v>-0.21</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -2695,7 +2789,7 @@
         <v>-1.26</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -2721,7 +2815,7 @@
         <v>1.33</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -2747,7 +2841,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -2773,7 +2867,7 @@
         <v>1.52</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -2799,7 +2893,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -2825,7 +2919,7 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -2851,7 +2945,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -2877,7 +2971,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -2903,7 +2997,7 @@
         <v>1.65</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -2929,7 +3023,7 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -2955,7 +3049,7 @@
         <v>-0.28999999999999998</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -2981,7 +3075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -3007,7 +3101,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -3033,7 +3127,7 @@
         <v>-0.7</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -3059,7 +3153,7 @@
         <v>-1.06</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>35</v>
       </c>
@@ -3085,7 +3179,7 @@
         <v>-0.24</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>36</v>
       </c>
@@ -3111,7 +3205,7 @@
         <v>0.48</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -3137,7 +3231,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -3163,7 +3257,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -3189,7 +3283,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -3215,7 +3309,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -3241,7 +3335,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -3267,7 +3361,7 @@
         <v>-0.04</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -3293,7 +3387,7 @@
         <v>-0.19</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -3319,7 +3413,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -3345,7 +3439,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -3371,7 +3465,7 @@
         <v>-1.93</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -3397,7 +3491,7 @@
         <v>-1.59</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -3423,7 +3517,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -3449,7 +3543,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -3475,7 +3569,7 @@
         <v>-0.44</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -3515,14 +3609,14 @@
       <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.19921875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.19921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>42</v>
       </c>
@@ -3542,7 +3636,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>92</v>
       </c>
@@ -3562,7 +3656,7 @@
         <v>1.85</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>93</v>
       </c>
@@ -3582,7 +3676,7 @@
         <v>1.99</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>94</v>
       </c>
@@ -3602,7 +3696,7 @@
         <v>1.68</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>95</v>
       </c>
@@ -3622,7 +3716,7 @@
         <v>2.3199999999999998</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>96</v>
       </c>
@@ -3642,7 +3736,7 @@
         <v>2.46</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>93</v>
       </c>
@@ -3662,7 +3756,7 @@
         <v>2.2400000000000002</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>97</v>
       </c>
@@ -3682,7 +3776,7 @@
         <v>2.58</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>98</v>
       </c>
@@ -3702,7 +3796,7 @@
         <v>2.4900000000000002</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>99</v>
       </c>
@@ -3722,7 +3816,7 @@
         <v>2.36</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>100</v>
       </c>
@@ -3742,7 +3836,7 @@
         <v>2.63</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>101</v>
       </c>
@@ -3762,7 +3856,7 @@
         <v>2.71</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>102</v>
       </c>
@@ -3782,7 +3876,7 @@
         <v>2.38</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>103</v>
       </c>
@@ -3802,7 +3896,7 @@
         <v>2.71</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>104</v>
       </c>
@@ -3822,7 +3916,7 @@
         <v>2.69</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>105</v>
       </c>
@@ -3842,7 +3936,7 @@
         <v>2.7</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>106</v>
       </c>
@@ -3862,7 +3956,7 @@
         <v>2.27</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>107</v>
       </c>
@@ -3882,7 +3976,7 @@
         <v>2.64</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>108</v>
       </c>
@@ -3902,7 +3996,7 @@
         <v>2.54</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>127</v>
       </c>
@@ -3922,7 +4016,7 @@
         <v>2.57</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>109</v>
       </c>
@@ -3942,7 +4036,7 @@
         <v>2.68</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>110</v>
       </c>
@@ -3962,7 +4056,7 @@
         <v>2.7</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>111</v>
       </c>
@@ -3982,7 +4076,7 @@
         <v>2.71</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>129</v>
       </c>
@@ -4002,7 +4096,7 @@
         <v>2.54</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>130</v>
       </c>
@@ -4022,7 +4116,7 @@
         <v>2.65</v>
       </c>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>112</v>
       </c>
@@ -4042,7 +4136,7 @@
         <v>2.37</v>
       </c>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>113</v>
       </c>
@@ -4062,7 +4156,7 @@
         <v>2.71</v>
       </c>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>114</v>
       </c>
@@ -4082,7 +4176,7 @@
         <v>1.87</v>
       </c>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>98</v>
       </c>
@@ -4102,7 +4196,7 @@
         <v>2.23</v>
       </c>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>115</v>
       </c>
@@ -4122,7 +4216,7 @@
         <v>2.69</v>
       </c>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="31" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>131</v>
       </c>
@@ -4142,7 +4236,7 @@
         <v>2.67</v>
       </c>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="32" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>116</v>
       </c>
@@ -4162,7 +4256,7 @@
         <v>2.66</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>117</v>
       </c>
@@ -4182,7 +4276,7 @@
         <v>2.68</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>118</v>
       </c>
@@ -4202,7 +4296,7 @@
         <v>2.56</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
         <v>119</v>
       </c>
@@ -4222,7 +4316,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>128</v>
       </c>
@@ -4242,7 +4336,7 @@
         <v>2.59</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
         <v>120</v>
       </c>
@@ -4262,7 +4356,7 @@
         <v>2.4300000000000002</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
         <v>121</v>
       </c>
@@ -4282,7 +4376,7 @@
         <v>2.4500000000000002</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
         <v>122</v>
       </c>
@@ -4302,7 +4396,7 @@
         <v>2.27</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
         <v>123</v>
       </c>
@@ -4322,7 +4416,7 @@
         <v>2.5499999999999998</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
         <v>124</v>
       </c>
@@ -4342,7 +4436,7 @@
         <v>2.14</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
         <v>125</v>
       </c>
@@ -4362,8 +4456,8 @@
         <v>2.12</v>
       </c>
     </row>
-    <row r="43" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="44" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>133</v>
       </c>
@@ -4378,7 +4472,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>134</v>
       </c>
@@ -4403,13 +4497,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8D7E26E-2B75-4FC8-A793-1D7462D1F2E7}">
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>42</v>
       </c>
@@ -4444,7 +4538,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>135</v>
       </c>
@@ -4479,7 +4573,7 @@
         <v>0.55100000000000005</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>135</v>
       </c>
@@ -4514,7 +4608,7 @@
         <v>0.77500000000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>136</v>
       </c>
@@ -4549,7 +4643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>137</v>
       </c>
@@ -4584,7 +4678,7 @@
         <v>0.60499999999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>138</v>
       </c>
@@ -4619,7 +4713,7 @@
         <v>2.9000000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>139</v>
       </c>
@@ -4654,7 +4748,7 @@
         <v>0.92200000000000004</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>140</v>
       </c>
@@ -4689,7 +4783,7 @@
         <v>1.7729999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>141</v>
       </c>
@@ -4724,7 +4818,7 @@
         <v>0.64700000000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>142</v>
       </c>
@@ -4759,7 +4853,7 @@
         <v>0.51800000000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>143</v>
       </c>
@@ -4794,7 +4888,7 @@
         <v>0.106</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>144</v>
       </c>
@@ -4829,7 +4923,7 @@
         <v>0.622</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>145</v>
       </c>
@@ -4864,7 +4958,7 @@
         <v>0.63800000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>146</v>
       </c>
@@ -4899,7 +4993,7 @@
         <v>0.85799999999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>147</v>
       </c>
@@ -4934,7 +5028,7 @@
         <v>0.58699999999999997</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>148</v>
       </c>
@@ -4969,7 +5063,7 @@
         <v>1.0009999999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>149</v>
       </c>

</xml_diff>

<commit_message>
updated csv and cma with altruism
</commit_message>
<xml_diff>
--- a/data/cumulative_ma_data.xlsx
+++ b/data/cumulative_ma_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rmata/Documents/GitHub/cumulative/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abagaini/Documents/PROJECTS/Cumul_MA/cumulative/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35077E81-9049-0946-AA62-D1EC3E32E4A3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BD8DC33-8669-E44D-BB6E-45331D9DECE6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13640" yWindow="600" windowWidth="34720" windowHeight="21340" xr2:uid="{D15F3EFF-771D-497D-BAA4-C31EA9079474}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="3" xr2:uid="{D15F3EFF-771D-497D-BAA4-C31EA9079474}"/>
   </bookViews>
   <sheets>
     <sheet name="Mata_et_al(2011)" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Seaman_et_al(2021)" sheetId="3" r:id="rId3"/>
     <sheet name="Sparrow_et_al(2021)" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="159">
   <si>
     <t>g_pos</t>
   </si>
@@ -426,123 +426,12 @@
     <t>Li (study 2)</t>
   </si>
   <si>
-    <t>Measure</t>
-  </si>
-  <si>
     <t>Fixed effect model</t>
   </si>
   <si>
     <t>Random effects model</t>
   </si>
   <si>
-    <t>Bailey et al.</t>
-  </si>
-  <si>
-    <t>Beadle et al.</t>
-  </si>
-  <si>
-    <t>Freund &amp; Blanchard-Fields</t>
-  </si>
-  <si>
-    <t>Gaesser et al.</t>
-  </si>
-  <si>
-    <t>Gong et al.</t>
-  </si>
-  <si>
-    <t>Hubbard et al.</t>
-  </si>
-  <si>
-    <t>Ojha &amp; Mishra</t>
-  </si>
-  <si>
-    <t>Pornpattananangkul et al.</t>
-  </si>
-  <si>
-    <t>Roalf et al.</t>
-  </si>
-  <si>
-    <t>Rosen et al.</t>
-  </si>
-  <si>
-    <t>Rosi et al.</t>
-  </si>
-  <si>
-    <t>Sparrow &amp; Spaniol (Exp 1)</t>
-  </si>
-  <si>
-    <t>Sparrow &amp; Spaniol (Exp 2)</t>
-  </si>
-  <si>
-    <t>Sparrow et al.</t>
-  </si>
-  <si>
-    <t>Sze et al.</t>
-  </si>
-  <si>
-    <t>Dictator Gaandme</t>
-  </si>
-  <si>
-    <t>Helping Tasandk</t>
-  </si>
-  <si>
-    <t>Donation</t>
-  </si>
-  <si>
-    <t>Willingness to Handelp</t>
-  </si>
-  <si>
-    <t>Social discounting</t>
-  </si>
-  <si>
-    <t>Gving choices factor</t>
-  </si>
-  <si>
-    <t>Altruism scale</t>
-  </si>
-  <si>
-    <t>Dictator game</t>
-  </si>
-  <si>
-    <t>Moral decision making</t>
-  </si>
-  <si>
-    <t>Altruistic intertemp. Choice</t>
-  </si>
-  <si>
-    <t>Self-report altruism scale</t>
-  </si>
-  <si>
-    <t>meth_Beh_vs_self-rep</t>
-  </si>
-  <si>
-    <t>meth_real_vs_hyp</t>
-  </si>
-  <si>
-    <t>meth_anon</t>
-  </si>
-  <si>
-    <t>20-40</t>
-  </si>
-  <si>
-    <t>Self-report</t>
-  </si>
-  <si>
-    <t>Real</t>
-  </si>
-  <si>
-    <t>Low</t>
-  </si>
-  <si>
-    <t>High</t>
-  </si>
-  <si>
-    <t>Beh</t>
-  </si>
-  <si>
-    <t>Hyp</t>
-  </si>
-  <si>
     <t>n</t>
   </si>
   <si>
@@ -562,15 +451,66 @@
   </si>
   <si>
     <t>58-80</t>
+  </si>
+  <si>
+    <t>se</t>
+  </si>
+  <si>
+    <t>beh_task</t>
+  </si>
+  <si>
+    <t>fin_task</t>
+  </si>
+  <si>
+    <t>Bailey</t>
+  </si>
+  <si>
+    <t>Bailey2</t>
+  </si>
+  <si>
+    <t>Beadle</t>
+  </si>
+  <si>
+    <t>Freund: Exp 4</t>
+  </si>
+  <si>
+    <t>Gaesser</t>
+  </si>
+  <si>
+    <t>Gong</t>
+  </si>
+  <si>
+    <t>Hubbard</t>
+  </si>
+  <si>
+    <t>Ojha</t>
+  </si>
+  <si>
+    <t>Pornpattananangkul</t>
+  </si>
+  <si>
+    <t>Rosen</t>
+  </si>
+  <si>
+    <t>Rosi</t>
+  </si>
+  <si>
+    <t>Sparrow: Exp 1</t>
+  </si>
+  <si>
+    <t>Sparrow: Exp 2</t>
+  </si>
+  <si>
+    <t>Sparrow: PNEC</t>
+  </si>
+  <si>
+    <t>Sze</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.000"/>
-  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -631,13 +571,9 @@
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -646,6 +582,10 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -962,8 +902,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38FBD286-E9F4-43DE-AE76-F152A62FC2EB}">
   <dimension ref="A1:R46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17:F32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -988,7 +928,7 @@
         <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>171</v>
+        <v>134</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>44</v>
@@ -1028,7 +968,7 @@
       <c r="E2" s="5">
         <v>16</v>
       </c>
-      <c r="F2" s="16">
+      <c r="F2" s="14">
         <f>D2+E2</f>
         <v>32</v>
       </c>
@@ -1074,7 +1014,7 @@
       <c r="E3" s="5">
         <v>39</v>
       </c>
-      <c r="F3" s="16">
+      <c r="F3" s="14">
         <f t="shared" ref="F3:F9" si="0">D3+E3</f>
         <v>78</v>
       </c>
@@ -1121,7 +1061,7 @@
       <c r="E4" s="5">
         <v>56</v>
       </c>
-      <c r="F4" s="16">
+      <c r="F4" s="14">
         <f t="shared" si="0"/>
         <v>119</v>
       </c>
@@ -1165,7 +1105,7 @@
       <c r="E5" s="5">
         <v>45</v>
       </c>
-      <c r="F5" s="16">
+      <c r="F5" s="14">
         <f t="shared" si="0"/>
         <v>86</v>
       </c>
@@ -1211,7 +1151,7 @@
       <c r="E6" s="5">
         <v>40</v>
       </c>
-      <c r="F6" s="16">
+      <c r="F6" s="14">
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
@@ -1258,7 +1198,7 @@
       <c r="E7" s="5">
         <v>79</v>
       </c>
-      <c r="F7" s="16">
+      <c r="F7" s="14">
         <f t="shared" si="0"/>
         <v>152</v>
       </c>
@@ -1305,7 +1245,7 @@
       <c r="E8" s="5">
         <v>18</v>
       </c>
-      <c r="F8" s="16">
+      <c r="F8" s="14">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
@@ -1351,7 +1291,7 @@
       <c r="E9" s="5">
         <v>52</v>
       </c>
-      <c r="F9" s="16">
+      <c r="F9" s="14">
         <f t="shared" si="0"/>
         <v>164</v>
       </c>
@@ -1532,7 +1472,7 @@
       <c r="E13" s="5">
         <v>24</v>
       </c>
-      <c r="F13" s="16">
+      <c r="F13" s="14">
         <f t="shared" ref="F13:F14" si="1">D13+E13</f>
         <v>48</v>
       </c>
@@ -1557,11 +1497,11 @@
       <c r="M13" s="2">
         <v>-0.39</v>
       </c>
-      <c r="N13" s="11"/>
+      <c r="N13" s="10"/>
       <c r="O13" s="2"/>
       <c r="P13" s="2"/>
-      <c r="Q13" s="11"/>
-      <c r="R13" s="11"/>
+      <c r="Q13" s="10"/>
+      <c r="R13" s="10"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -1579,7 +1519,7 @@
       <c r="E14" s="5">
         <v>40</v>
       </c>
-      <c r="F14" s="16">
+      <c r="F14" s="14">
         <f t="shared" si="1"/>
         <v>80</v>
       </c>
@@ -1625,10 +1565,10 @@
         <v>80</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>174</v>
+        <v>137</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>176</v>
+        <v>139</v>
       </c>
       <c r="I15" s="2" t="s">
         <v>41</v>
@@ -1666,10 +1606,10 @@
         <v>106</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>175</v>
+        <v>138</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>177</v>
+        <v>140</v>
       </c>
       <c r="I16" s="2" t="s">
         <v>41</v>
@@ -1708,7 +1648,7 @@
       <c r="E17" s="5">
         <v>20</v>
       </c>
-      <c r="F17" s="16">
+      <c r="F17" s="14">
         <f t="shared" ref="F17:F32" si="2">D17+E17</f>
         <v>43</v>
       </c>
@@ -1752,7 +1692,7 @@
       <c r="E18" s="5">
         <v>23</v>
       </c>
-      <c r="F18" s="16">
+      <c r="F18" s="14">
         <f t="shared" si="2"/>
         <v>49</v>
       </c>
@@ -1798,7 +1738,7 @@
       <c r="E19" s="5">
         <v>9</v>
       </c>
-      <c r="F19" s="16">
+      <c r="F19" s="14">
         <f t="shared" si="2"/>
         <v>21</v>
       </c>
@@ -1845,7 +1785,7 @@
       <c r="E20" s="5">
         <v>30</v>
       </c>
-      <c r="F20" s="16">
+      <c r="F20" s="14">
         <f t="shared" si="2"/>
         <v>60</v>
       </c>
@@ -1889,7 +1829,7 @@
       <c r="E21" s="5">
         <v>58</v>
       </c>
-      <c r="F21" s="16">
+      <c r="F21" s="14">
         <f t="shared" si="2"/>
         <v>116</v>
       </c>
@@ -1933,7 +1873,7 @@
       <c r="E22" s="5">
         <v>22</v>
       </c>
-      <c r="F22" s="16">
+      <c r="F22" s="14">
         <f t="shared" si="2"/>
         <v>44</v>
       </c>
@@ -1979,7 +1919,7 @@
       <c r="E23" s="5">
         <v>45</v>
       </c>
-      <c r="F23" s="16">
+      <c r="F23" s="14">
         <f t="shared" si="2"/>
         <v>87</v>
       </c>
@@ -2025,7 +1965,7 @@
       <c r="E24" s="5">
         <v>53</v>
       </c>
-      <c r="F24" s="16">
+      <c r="F24" s="14">
         <f t="shared" si="2"/>
         <v>103</v>
       </c>
@@ -2072,7 +2012,7 @@
       <c r="E25" s="5">
         <v>44</v>
       </c>
-      <c r="F25" s="16">
+      <c r="F25" s="14">
         <f t="shared" si="2"/>
         <v>84</v>
       </c>
@@ -2116,7 +2056,7 @@
       <c r="E26" s="5">
         <v>192</v>
       </c>
-      <c r="F26" s="16">
+      <c r="F26" s="14">
         <f t="shared" si="2"/>
         <v>384</v>
       </c>
@@ -2163,7 +2103,7 @@
       <c r="E27" s="5">
         <v>42</v>
       </c>
-      <c r="F27" s="16">
+      <c r="F27" s="14">
         <f t="shared" si="2"/>
         <v>77</v>
       </c>
@@ -2210,7 +2150,7 @@
       <c r="E28" s="5">
         <v>59</v>
       </c>
-      <c r="F28" s="16">
+      <c r="F28" s="14">
         <f t="shared" si="2"/>
         <v>108</v>
       </c>
@@ -2255,7 +2195,7 @@
       <c r="E29" s="5">
         <v>24</v>
       </c>
-      <c r="F29" s="16">
+      <c r="F29" s="14">
         <f t="shared" si="2"/>
         <v>75</v>
       </c>
@@ -2300,7 +2240,7 @@
       <c r="E30" s="5">
         <v>168</v>
       </c>
-      <c r="F30" s="16">
+      <c r="F30" s="14">
         <f t="shared" si="2"/>
         <v>829</v>
       </c>
@@ -2344,7 +2284,7 @@
       <c r="E31" s="5">
         <v>61</v>
       </c>
-      <c r="F31" s="16">
+      <c r="F31" s="14">
         <f t="shared" si="2"/>
         <v>419</v>
       </c>
@@ -2391,7 +2331,7 @@
       <c r="E32" s="5">
         <v>63</v>
       </c>
-      <c r="F32" s="16">
+      <c r="F32" s="14">
         <f t="shared" si="2"/>
         <v>150</v>
       </c>
@@ -2437,7 +2377,7 @@
       <c r="E33" s="5">
         <v>52</v>
       </c>
-      <c r="F33" s="13">
+      <c r="F33" s="11">
         <v>85</v>
       </c>
       <c r="G33" s="4">
@@ -2455,10 +2395,10 @@
       <c r="K33" s="2">
         <v>0.76</v>
       </c>
-      <c r="L33" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="M33" s="14" t="s">
+      <c r="L33" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="M33" s="12" t="s">
         <v>41</v>
       </c>
     </row>
@@ -2469,7 +2409,7 @@
       <c r="B34">
         <v>2008</v>
       </c>
-      <c r="C34" s="13" t="s">
+      <c r="C34" s="11" t="s">
         <v>72</v>
       </c>
       <c r="D34" s="5">
@@ -2478,7 +2418,7 @@
       <c r="E34" s="5">
         <v>52</v>
       </c>
-      <c r="F34" s="13">
+      <c r="F34" s="11">
         <v>85</v>
       </c>
       <c r="G34" s="4">
@@ -2493,154 +2433,154 @@
       <c r="J34" s="2">
         <v>10.4</v>
       </c>
-      <c r="K34" s="15">
+      <c r="K34" s="13">
         <v>0.19</v>
       </c>
-      <c r="L34" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="M34" s="14" t="s">
+      <c r="L34" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="M34" s="12" t="s">
         <v>41</v>
       </c>
       <c r="O34" s="9"/>
     </row>
-    <row r="35" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="36" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="37" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="38" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="13"/>
-      <c r="B38" s="13"/>
-      <c r="C38" s="13"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="13"/>
-      <c r="F38" s="13"/>
-      <c r="G38" s="13"/>
-      <c r="H38" s="13"/>
-      <c r="I38" s="13"/>
-      <c r="J38" s="13"/>
-      <c r="K38" s="13"/>
-      <c r="L38" s="13"/>
-      <c r="M38" s="13"/>
+      <c r="A38" s="11"/>
+      <c r="B38" s="11"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="11"/>
+      <c r="G38" s="11"/>
+      <c r="H38" s="11"/>
+      <c r="I38" s="11"/>
+      <c r="J38" s="11"/>
+      <c r="K38" s="11"/>
+      <c r="L38" s="11"/>
+      <c r="M38" s="11"/>
     </row>
     <row r="39" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="13"/>
-      <c r="B39" s="13"/>
-      <c r="C39" s="13"/>
-      <c r="D39" s="13"/>
-      <c r="E39" s="13"/>
-      <c r="F39" s="13"/>
-      <c r="G39" s="13"/>
-      <c r="H39" s="13"/>
-      <c r="I39" s="13"/>
-      <c r="J39" s="13"/>
-      <c r="K39" s="13"/>
-      <c r="L39" s="13"/>
-      <c r="M39" s="13"/>
+      <c r="A39" s="11"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="11"/>
+      <c r="H39" s="11"/>
+      <c r="I39" s="11"/>
+      <c r="J39" s="11"/>
+      <c r="K39" s="11"/>
+      <c r="L39" s="11"/>
+      <c r="M39" s="11"/>
     </row>
     <row r="40" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="13"/>
-      <c r="B40" s="13"/>
-      <c r="C40" s="13"/>
-      <c r="D40" s="13"/>
-      <c r="E40" s="13"/>
-      <c r="F40" s="13"/>
-      <c r="G40" s="13"/>
-      <c r="H40" s="13"/>
-      <c r="I40" s="13"/>
-      <c r="J40" s="13"/>
-      <c r="K40" s="13"/>
-      <c r="L40" s="13"/>
-      <c r="M40" s="13"/>
+      <c r="A40" s="11"/>
+      <c r="B40" s="11"/>
+      <c r="C40" s="11"/>
+      <c r="D40" s="11"/>
+      <c r="E40" s="11"/>
+      <c r="F40" s="11"/>
+      <c r="G40" s="11"/>
+      <c r="H40" s="11"/>
+      <c r="I40" s="11"/>
+      <c r="J40" s="11"/>
+      <c r="K40" s="11"/>
+      <c r="L40" s="11"/>
+      <c r="M40" s="11"/>
     </row>
     <row r="41" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="13"/>
-      <c r="B41" s="13"/>
-      <c r="C41" s="13"/>
-      <c r="D41" s="13"/>
-      <c r="E41" s="13"/>
-      <c r="F41" s="13"/>
-      <c r="G41" s="13"/>
-      <c r="H41" s="13"/>
-      <c r="I41" s="13"/>
-      <c r="J41" s="13"/>
-      <c r="K41" s="13"/>
-      <c r="L41" s="13"/>
-      <c r="M41" s="13"/>
+      <c r="A41" s="11"/>
+      <c r="B41" s="11"/>
+      <c r="C41" s="11"/>
+      <c r="D41" s="11"/>
+      <c r="E41" s="11"/>
+      <c r="F41" s="11"/>
+      <c r="G41" s="11"/>
+      <c r="H41" s="11"/>
+      <c r="I41" s="11"/>
+      <c r="J41" s="11"/>
+      <c r="K41" s="11"/>
+      <c r="L41" s="11"/>
+      <c r="M41" s="11"/>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A42" s="13"/>
-      <c r="B42" s="13"/>
-      <c r="C42" s="13"/>
-      <c r="D42" s="13"/>
-      <c r="E42" s="13"/>
-      <c r="F42" s="13"/>
-      <c r="G42" s="13"/>
-      <c r="H42" s="13"/>
-      <c r="I42" s="13"/>
-      <c r="J42" s="13"/>
-      <c r="K42" s="13"/>
-      <c r="L42" s="13"/>
-      <c r="M42" s="13"/>
+      <c r="A42" s="11"/>
+      <c r="B42" s="11"/>
+      <c r="C42" s="11"/>
+      <c r="D42" s="11"/>
+      <c r="E42" s="11"/>
+      <c r="F42" s="11"/>
+      <c r="G42" s="11"/>
+      <c r="H42" s="11"/>
+      <c r="I42" s="11"/>
+      <c r="J42" s="11"/>
+      <c r="K42" s="11"/>
+      <c r="L42" s="11"/>
+      <c r="M42" s="11"/>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A43" s="13"/>
-      <c r="B43" s="13"/>
-      <c r="C43" s="13"/>
-      <c r="D43" s="13"/>
-      <c r="E43" s="13"/>
-      <c r="F43" s="13"/>
-      <c r="G43" s="13"/>
-      <c r="H43" s="13"/>
-      <c r="I43" s="13"/>
-      <c r="J43" s="13"/>
-      <c r="K43" s="13"/>
-      <c r="L43" s="13"/>
-      <c r="M43" s="13"/>
+      <c r="A43" s="11"/>
+      <c r="B43" s="11"/>
+      <c r="C43" s="11"/>
+      <c r="D43" s="11"/>
+      <c r="E43" s="11"/>
+      <c r="F43" s="11"/>
+      <c r="G43" s="11"/>
+      <c r="H43" s="11"/>
+      <c r="I43" s="11"/>
+      <c r="J43" s="11"/>
+      <c r="K43" s="11"/>
+      <c r="L43" s="11"/>
+      <c r="M43" s="11"/>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A44" s="13"/>
-      <c r="B44" s="13"/>
-      <c r="C44" s="13"/>
-      <c r="D44" s="13"/>
-      <c r="E44" s="13"/>
-      <c r="F44" s="13"/>
-      <c r="G44" s="13"/>
-      <c r="H44" s="13"/>
-      <c r="I44" s="13"/>
-      <c r="J44" s="13"/>
-      <c r="K44" s="13"/>
-      <c r="L44" s="13"/>
-      <c r="M44" s="13"/>
+      <c r="A44" s="11"/>
+      <c r="B44" s="11"/>
+      <c r="C44" s="11"/>
+      <c r="D44" s="11"/>
+      <c r="E44" s="11"/>
+      <c r="F44" s="11"/>
+      <c r="G44" s="11"/>
+      <c r="H44" s="11"/>
+      <c r="I44" s="11"/>
+      <c r="J44" s="11"/>
+      <c r="K44" s="11"/>
+      <c r="L44" s="11"/>
+      <c r="M44" s="11"/>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A45" s="13"/>
-      <c r="B45" s="13"/>
-      <c r="C45" s="13"/>
-      <c r="D45" s="13"/>
-      <c r="E45" s="13"/>
-      <c r="F45" s="13"/>
-      <c r="G45" s="13"/>
-      <c r="H45" s="13"/>
-      <c r="I45" s="13"/>
-      <c r="J45" s="13"/>
-      <c r="K45" s="13"/>
-      <c r="L45" s="13"/>
-      <c r="M45" s="13"/>
+      <c r="A45" s="11"/>
+      <c r="B45" s="11"/>
+      <c r="C45" s="11"/>
+      <c r="D45" s="11"/>
+      <c r="E45" s="11"/>
+      <c r="F45" s="11"/>
+      <c r="G45" s="11"/>
+      <c r="H45" s="11"/>
+      <c r="I45" s="11"/>
+      <c r="J45" s="11"/>
+      <c r="K45" s="11"/>
+      <c r="L45" s="11"/>
+      <c r="M45" s="11"/>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A46" s="13"/>
-      <c r="B46" s="13"/>
-      <c r="C46" s="13"/>
-      <c r="D46" s="13"/>
-      <c r="E46" s="13"/>
-      <c r="F46" s="13"/>
-      <c r="G46" s="13"/>
-      <c r="H46" s="13"/>
-      <c r="I46" s="13"/>
-      <c r="J46" s="13"/>
-      <c r="K46" s="13"/>
-      <c r="L46" s="13"/>
-      <c r="M46" s="13"/>
+      <c r="A46" s="11"/>
+      <c r="B46" s="11"/>
+      <c r="C46" s="11"/>
+      <c r="D46" s="11"/>
+      <c r="E46" s="11"/>
+      <c r="F46" s="11"/>
+      <c r="G46" s="11"/>
+      <c r="H46" s="11"/>
+      <c r="I46" s="11"/>
+      <c r="J46" s="11"/>
+      <c r="K46" s="11"/>
+      <c r="L46" s="11"/>
+      <c r="M46" s="11"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -3630,10 +3570,10 @@
         <v>91</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>172</v>
+        <v>135</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>173</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="2:7" x14ac:dyDescent="0.2">
@@ -4459,7 +4399,7 @@
     <row r="43" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="44" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D44" s="7">
         <f>SUBTOTAL(9,D2:D42)</f>
@@ -4474,7 +4414,7 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -4497,13 +4437,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8D7E26E-2B75-4FC8-A793-1D7462D1F2E7}">
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>42</v>
       </c>
@@ -4511,13 +4451,13 @@
         <v>43</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>132</v>
+        <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>5</v>
+        <v>134</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>44</v>
@@ -4526,576 +4466,519 @@
         <v>68</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>162</v>
+        <v>91</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>141</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>91</v>
+        <v>142</v>
+      </c>
+      <c r="K1" s="15" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="B2">
         <v>2013</v>
       </c>
-      <c r="C2" t="s">
-        <v>150</v>
-      </c>
-      <c r="D2" s="10">
+      <c r="C2">
         <v>35</v>
       </c>
-      <c r="E2" s="10">
+      <c r="D2">
         <v>34</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2">
         <v>21.3</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2">
         <v>73.900000000000006</v>
       </c>
-      <c r="H2" t="s">
-        <v>169</v>
-      </c>
-      <c r="I2" t="s">
-        <v>170</v>
-      </c>
-      <c r="J2" t="s">
-        <v>167</v>
-      </c>
-      <c r="K2" s="12">
-        <v>0.55100000000000005</v>
+      <c r="H2">
+        <v>0.55121340239401695</v>
+      </c>
+      <c r="I2">
+        <v>0.24267103671162901</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>135</v>
+        <v>145</v>
       </c>
       <c r="B3">
         <v>2018</v>
       </c>
-      <c r="C3" t="s">
-        <v>151</v>
-      </c>
-      <c r="D3" s="10">
+      <c r="C3">
         <v>40</v>
       </c>
-      <c r="E3" s="10">
+      <c r="D3">
         <v>39</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3">
         <v>19.88</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3">
         <v>72.44</v>
       </c>
-      <c r="H3" t="s">
-        <v>169</v>
-      </c>
-      <c r="I3" t="s">
-        <v>166</v>
-      </c>
-      <c r="J3" t="s">
-        <v>167</v>
-      </c>
-      <c r="K3" s="12">
-        <v>0.77500000000000002</v>
+      <c r="H3">
+        <v>0.77471963925238896</v>
+      </c>
+      <c r="I3">
+        <v>0.23120296003369001</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>136</v>
+        <v>146</v>
       </c>
       <c r="B4">
-        <v>2015</v>
-      </c>
-      <c r="C4" t="s">
-        <v>150</v>
-      </c>
-      <c r="D4" s="10">
+        <v>2013</v>
+      </c>
+      <c r="C4">
         <v>24</v>
       </c>
-      <c r="E4" s="10">
+      <c r="D4">
         <v>24</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4">
         <v>19.829999999999998</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4">
         <v>77.92</v>
       </c>
-      <c r="H4" t="s">
-        <v>169</v>
-      </c>
-      <c r="I4" t="s">
-        <v>166</v>
-      </c>
-      <c r="J4" t="s">
-        <v>168</v>
-      </c>
-      <c r="K4" s="12">
+      <c r="H4">
         <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0.28394275533916002</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="B5">
         <v>2014</v>
       </c>
-      <c r="C5" t="s">
-        <v>152</v>
-      </c>
-      <c r="D5" s="10">
-        <v>48</v>
-      </c>
-      <c r="E5" s="10">
-        <v>69</v>
-      </c>
-      <c r="F5" s="2">
+      <c r="E5">
+        <v>117</v>
+      </c>
+      <c r="F5">
         <v>24.1</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5">
         <v>68.8</v>
       </c>
-      <c r="H5" t="s">
-        <v>169</v>
-      </c>
-      <c r="I5" t="s">
-        <v>166</v>
-      </c>
-      <c r="J5" t="s">
-        <v>168</v>
-      </c>
-      <c r="K5" s="12">
-        <v>0.60499999999999998</v>
+      <c r="H5">
+        <v>0.60542691683972105</v>
+      </c>
+      <c r="I5">
+        <v>0.19454005685892301</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="B6">
         <v>2017</v>
       </c>
-      <c r="C6" t="s">
-        <v>153</v>
-      </c>
-      <c r="D6" s="10">
+      <c r="C6">
         <v>30</v>
       </c>
-      <c r="E6" s="10">
+      <c r="D6">
         <v>30</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6">
         <v>21.97</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6">
         <v>73.63</v>
       </c>
-      <c r="H6" t="s">
-        <v>165</v>
-      </c>
-      <c r="I6" t="s">
-        <v>170</v>
-      </c>
-      <c r="J6" t="s">
-        <v>167</v>
-      </c>
-      <c r="K6" s="12">
-        <v>2.9000000000000001E-2</v>
+      <c r="H6" s="16">
+        <v>2.9002292479318501E-2</v>
+      </c>
+      <c r="I6">
+        <v>0.25485940936830698</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="B7">
         <v>2019</v>
       </c>
-      <c r="C7" t="s">
-        <v>154</v>
-      </c>
-      <c r="D7" s="10">
+      <c r="C7">
         <v>89</v>
       </c>
-      <c r="E7" s="10">
+      <c r="D7">
         <v>66</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7">
         <v>30.12</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7">
         <v>69.39</v>
       </c>
-      <c r="H7" t="s">
-        <v>169</v>
-      </c>
-      <c r="I7" t="s">
-        <v>170</v>
-      </c>
-      <c r="J7" t="s">
-        <v>167</v>
-      </c>
-      <c r="K7" s="12">
-        <v>0.92200000000000004</v>
+      <c r="H7">
+        <v>0.92185272462318801</v>
+      </c>
+      <c r="I7">
+        <v>0.169912662071317</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="B8">
         <v>2016</v>
       </c>
-      <c r="C8" t="s">
-        <v>155</v>
-      </c>
-      <c r="D8" s="10">
+      <c r="C8">
         <v>19</v>
       </c>
-      <c r="E8" s="10">
+      <c r="D8">
         <v>5</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8">
         <v>27.95</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8">
         <v>63</v>
       </c>
-      <c r="H8" t="s">
-        <v>169</v>
-      </c>
-      <c r="I8" t="s">
-        <v>166</v>
-      </c>
-      <c r="J8" t="s">
-        <v>168</v>
-      </c>
-      <c r="K8" s="12">
-        <v>1.7729999999999999</v>
+      <c r="H8">
+        <v>1.77251240478261</v>
+      </c>
+      <c r="I8">
+        <v>0.54860120037934201</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>141</v>
+        <v>151</v>
       </c>
       <c r="B9">
         <v>2014</v>
       </c>
-      <c r="C9" t="s">
-        <v>156</v>
-      </c>
-      <c r="D9" s="10">
+      <c r="C9">
         <v>180</v>
       </c>
-      <c r="E9" s="10">
+      <c r="D9">
         <v>180</v>
       </c>
-      <c r="F9" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="H9" t="s">
-        <v>165</v>
-      </c>
-      <c r="I9" t="s">
-        <v>170</v>
-      </c>
-      <c r="J9" t="s">
-        <v>167</v>
-      </c>
-      <c r="K9" s="12">
-        <v>0.64700000000000002</v>
+      <c r="H9">
+        <v>0.64710247092879902</v>
+      </c>
+      <c r="I9">
+        <v>0.107917366737087</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>142</v>
+        <v>152</v>
       </c>
       <c r="B10">
-        <v>2019</v>
-      </c>
-      <c r="C10" t="s">
-        <v>154</v>
-      </c>
-      <c r="D10" s="10">
+        <v>2017</v>
+      </c>
+      <c r="C10">
         <v>39</v>
       </c>
-      <c r="E10" s="10">
+      <c r="D10">
         <v>39</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10">
         <v>22.79</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10">
         <v>69.69</v>
       </c>
-      <c r="H10" t="s">
-        <v>169</v>
-      </c>
-      <c r="I10" t="s">
-        <v>170</v>
-      </c>
-      <c r="J10" t="s">
-        <v>167</v>
-      </c>
-      <c r="K10" s="12">
-        <v>0.51800000000000002</v>
+      <c r="H10">
+        <v>0.518264161225095</v>
+      </c>
+      <c r="I10">
+        <v>0.22802055316810399</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>143</v>
+        <v>122</v>
       </c>
       <c r="B11">
         <v>2012</v>
       </c>
-      <c r="C11" t="s">
-        <v>157</v>
-      </c>
-      <c r="D11" s="10">
+      <c r="C11">
         <v>29</v>
       </c>
-      <c r="E11" s="10">
+      <c r="D11">
         <v>30</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11">
         <v>30.14</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G11">
         <v>71.3</v>
       </c>
-      <c r="H11" t="s">
-        <v>169</v>
-      </c>
-      <c r="I11" t="s">
-        <v>166</v>
-      </c>
-      <c r="J11" t="s">
-        <v>168</v>
-      </c>
-      <c r="K11" s="12">
-        <v>0.106</v>
+      <c r="H11">
+        <v>0.10622410902187</v>
+      </c>
+      <c r="I11">
+        <v>0.25715960845099101</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
       <c r="B12">
         <v>2016</v>
       </c>
-      <c r="C12" t="s">
-        <v>158</v>
-      </c>
-      <c r="D12" s="10">
+      <c r="C12">
         <v>74</v>
       </c>
-      <c r="E12" s="10">
+      <c r="D12">
         <v>33</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12">
         <v>26.42</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G12">
         <v>71.459999999999994</v>
       </c>
-      <c r="H12" t="s">
-        <v>165</v>
-      </c>
-      <c r="I12" t="s">
-        <v>170</v>
-      </c>
-      <c r="J12" t="s">
-        <v>167</v>
-      </c>
-      <c r="K12" s="12">
-        <v>0.622</v>
+      <c r="H12">
+        <v>0.62165257563899101</v>
+      </c>
+      <c r="I12">
+        <v>0.21212542424803399</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
       <c r="B13">
         <v>2019</v>
       </c>
-      <c r="C13" t="s">
-        <v>157</v>
-      </c>
-      <c r="D13" s="10">
+      <c r="C13">
         <v>48</v>
       </c>
-      <c r="E13" s="10">
+      <c r="D13">
         <v>48</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13">
         <v>23.29</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G13">
         <v>70.19</v>
       </c>
-      <c r="H13" t="s">
-        <v>169</v>
-      </c>
-      <c r="I13" t="s">
-        <v>170</v>
-      </c>
-      <c r="J13" t="s">
-        <v>168</v>
-      </c>
-      <c r="K13" s="12">
-        <v>0.63800000000000001</v>
+      <c r="H13">
+        <v>0.63819418586767596</v>
+      </c>
+      <c r="I13">
+        <v>0.207663136409207</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
+      <c r="K13">
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="B14">
         <v>2018</v>
       </c>
-      <c r="C14" t="s">
-        <v>159</v>
-      </c>
-      <c r="D14" s="10">
+      <c r="C14">
         <v>32</v>
       </c>
-      <c r="E14" s="10">
+      <c r="D14">
         <v>30</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14">
         <v>25.28</v>
       </c>
-      <c r="G14" s="2">
+      <c r="G14">
         <v>70.569999999999993</v>
       </c>
-      <c r="H14" t="s">
-        <v>169</v>
-      </c>
-      <c r="I14" t="s">
-        <v>166</v>
-      </c>
-      <c r="J14" t="s">
-        <v>167</v>
-      </c>
-      <c r="K14" s="12">
-        <v>0.85799999999999998</v>
+      <c r="H14">
+        <v>0.858350729706717</v>
+      </c>
+      <c r="I14">
+        <v>0.26251444013359798</v>
+      </c>
+      <c r="J14">
+        <v>1</v>
+      </c>
+      <c r="K14">
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
       <c r="B15">
         <v>2018</v>
       </c>
-      <c r="C15" t="s">
-        <v>159</v>
-      </c>
-      <c r="D15" s="10">
+      <c r="C15">
         <v>31</v>
       </c>
-      <c r="E15" s="10">
+      <c r="D15">
         <v>23</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15">
         <v>20.84</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G15">
         <v>71.349999999999994</v>
       </c>
-      <c r="H15" t="s">
-        <v>169</v>
-      </c>
-      <c r="I15" t="s">
-        <v>166</v>
-      </c>
-      <c r="J15" t="s">
-        <v>168</v>
-      </c>
-      <c r="K15" s="12">
-        <v>0.58699999999999997</v>
+      <c r="H15">
+        <v>0.58748392533682103</v>
+      </c>
+      <c r="I15">
+        <v>0.27704276483588702</v>
+      </c>
+      <c r="J15">
+        <v>1</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
       <c r="B16">
         <v>2019</v>
       </c>
-      <c r="C16" t="s">
-        <v>160</v>
-      </c>
-      <c r="D16" s="10">
+      <c r="C16">
         <v>36</v>
       </c>
-      <c r="E16" s="10">
+      <c r="D16">
         <v>36</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16">
         <v>21</v>
       </c>
-      <c r="G16" s="2">
+      <c r="G16">
         <v>70.11</v>
       </c>
-      <c r="H16" t="s">
-        <v>165</v>
-      </c>
-      <c r="I16" t="s">
-        <v>166</v>
-      </c>
-      <c r="J16" t="s">
-        <v>167</v>
-      </c>
-      <c r="K16" s="12">
-        <v>1.0009999999999999</v>
+      <c r="H16">
+        <v>1.00095479248103</v>
+      </c>
+      <c r="I16">
+        <v>0.24763874405547101</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
       <c r="B17">
         <v>2012</v>
       </c>
-      <c r="C17" t="s">
-        <v>152</v>
-      </c>
-      <c r="D17" s="10">
+      <c r="C17">
         <v>71</v>
       </c>
-      <c r="E17" s="10">
+      <c r="D17">
         <v>70</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F17">
         <v>23.07</v>
       </c>
-      <c r="G17" s="2">
+      <c r="G17">
         <v>66.430000000000007</v>
       </c>
-      <c r="H17" t="s">
-        <v>169</v>
-      </c>
-      <c r="I17" t="s">
-        <v>166</v>
-      </c>
-      <c r="J17" t="s">
-        <v>168</v>
-      </c>
-      <c r="K17" s="12">
-        <v>0.52900000000000003</v>
+      <c r="H17">
+        <v>0.52918123403528905</v>
+      </c>
+      <c r="I17">
+        <v>0.17046222221447099</v>
+      </c>
+      <c r="J17">
+        <v>1</v>
+      </c>
+      <c r="K17">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated risk, time and altruism scripts, figs and data
created/edited scripts for cma by study and year + basic ma
created figures
attempted to calculate SEs for g when missing
</commit_message>
<xml_diff>
--- a/data/cumulative_ma_data.xlsx
+++ b/data/cumulative_ma_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abagaini/Documents/PROJECTS/Cumul_MA/cumulative/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BD8DC33-8669-E44D-BB6E-45331D9DECE6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB850629-CC27-2F4D-9730-56950F7143B7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="3" xr2:uid="{D15F3EFF-771D-497D-BAA4-C31EA9079474}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17060" xr2:uid="{D15F3EFF-771D-497D-BAA4-C31EA9079474}"/>
   </bookViews>
   <sheets>
     <sheet name="Mata_et_al(2011)" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="163">
   <si>
     <t>g_pos</t>
   </si>
@@ -153,9 +153,6 @@
     <t>Large</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>Source</t>
   </si>
   <si>
@@ -505,6 +502,21 @@
   </si>
   <si>
     <t>Sze</t>
+  </si>
+  <si>
+    <t>se_pos</t>
+  </si>
+  <si>
+    <t>se_neg</t>
+  </si>
+  <si>
+    <t>se_all</t>
+  </si>
+  <si>
+    <t>se_gains</t>
+  </si>
+  <si>
+    <t>se_losses</t>
   </si>
 </sst>
 </file>
@@ -554,7 +566,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -570,7 +582,6 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -902,8 +913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38FBD286-E9F4-43DE-AE76-F152A62FC2EB}">
   <dimension ref="A1:R46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -913,13 +924,13 @@
   <sheetData>
     <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -928,39 +939,48 @@
         <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="K1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>89</v>
+      <c r="N1" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B2">
         <v>2003</v>
       </c>
       <c r="C2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D2" s="5">
         <v>16</v>
@@ -968,7 +988,7 @@
       <c r="E2" s="5">
         <v>16</v>
       </c>
-      <c r="F2" s="14">
+      <c r="F2" s="13">
         <f>D2+E2</f>
         <v>32</v>
       </c>
@@ -978,35 +998,30 @@
       <c r="H2" s="4">
         <v>75</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>41</v>
-      </c>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
       <c r="K2" s="2">
         <v>0.06</v>
       </c>
-      <c r="L2" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="N2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2">
+        <f>SQRT((D2+E2)/(D2*E2)+K2^2/(2*(D2+E2)))</f>
+        <v>0.35363293115885008</v>
+      </c>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B3">
         <v>2010</v>
       </c>
       <c r="C3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D3" s="5">
         <v>39</v>
@@ -1014,33 +1029,27 @@
       <c r="E3" s="5">
         <v>39</v>
       </c>
-      <c r="F3" s="14">
+      <c r="F3" s="13">
         <f t="shared" ref="F3:F9" si="0">D3+E3</f>
         <v>78</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>41</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
       <c r="K3" s="2">
         <v>1.72</v>
       </c>
-      <c r="L3" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2">
+        <f t="shared" ref="N3:N34" si="1">SQRT((D3+E3)/(D3*E3)+K3^2/(2*(D3+E3)))</f>
+        <v>0.26503990991198634</v>
+      </c>
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
@@ -1053,7 +1062,7 @@
         <v>2007</v>
       </c>
       <c r="C4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D4" s="5">
         <v>63</v>
@@ -1061,7 +1070,7 @@
       <c r="E4" s="5">
         <v>56</v>
       </c>
-      <c r="F4" s="14">
+      <c r="F4" s="13">
         <f t="shared" si="0"/>
         <v>119</v>
       </c>
@@ -1071,12 +1080,8 @@
       <c r="H4" s="4">
         <v>76.7</v>
       </c>
-      <c r="I4" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>41</v>
-      </c>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
       <c r="K4" s="2">
         <v>0.19</v>
       </c>
@@ -1086,18 +1091,28 @@
       <c r="M4" s="2">
         <v>0</v>
       </c>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
+      <c r="N4" s="2">
+        <f t="shared" si="1"/>
+        <v>0.18407020237514718</v>
+      </c>
+      <c r="O4">
+        <f t="shared" ref="O4:O31" si="2">SQRT((D4+E4)/(D4*E4)+L4^2/(2*(D4+E4)))</f>
+        <v>0.18391491659265916</v>
+      </c>
+      <c r="P4" s="2">
+        <f t="shared" ref="P4:P31" si="3">SQRT((D4+E4)/(D4*E4)+M4^2/(2*(D4+E4)))</f>
+        <v>0.18365772167311323</v>
+      </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B5">
         <v>2004</v>
       </c>
       <c r="C5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D5" s="5">
         <v>41</v>
@@ -1105,45 +1120,40 @@
       <c r="E5" s="5">
         <v>45</v>
       </c>
-      <c r="F5" s="14">
+      <c r="F5" s="13">
         <f t="shared" si="0"/>
         <v>86</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>41</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
       <c r="K5" s="2">
         <v>0.31</v>
       </c>
-      <c r="L5" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2">
+        <f t="shared" si="1"/>
+        <v>0.21718928853627611</v>
+      </c>
+      <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B6">
         <v>2005</v>
       </c>
       <c r="C6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D6" s="5">
         <v>40</v>
@@ -1151,46 +1161,40 @@
       <c r="E6" s="5">
         <v>40</v>
       </c>
-      <c r="F6" s="14">
+      <c r="F6" s="13">
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>41</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
       <c r="K6" s="2">
         <v>2.72</v>
       </c>
-      <c r="L6" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2">
+        <f t="shared" si="1"/>
+        <v>0.31022572427185985</v>
+      </c>
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
       <c r="R6" s="2"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B7">
         <v>2009</v>
       </c>
       <c r="C7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D7" s="5">
         <v>73</v>
@@ -1198,7 +1202,7 @@
       <c r="E7" s="5">
         <v>79</v>
       </c>
-      <c r="F7" s="14">
+      <c r="F7" s="13">
         <f t="shared" si="0"/>
         <v>152</v>
       </c>
@@ -1217,27 +1221,25 @@
       <c r="K7" s="2">
         <v>0.48</v>
       </c>
-      <c r="L7" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="M7" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2">
+        <f t="shared" si="1"/>
+        <v>0.16466557843681137</v>
+      </c>
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B8">
         <v>1998</v>
       </c>
       <c r="C8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D8" s="5">
         <v>18</v>
@@ -1245,45 +1247,40 @@
       <c r="E8" s="5">
         <v>18</v>
       </c>
-      <c r="F8" s="14">
+      <c r="F8" s="13">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>41</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
       <c r="K8" s="2">
         <v>-0.45</v>
       </c>
-      <c r="L8" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="M8" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="N8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2">
+        <f t="shared" si="1"/>
+        <v>0.33752571918464391</v>
+      </c>
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
       <c r="R8" s="2"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B9">
         <v>2010</v>
       </c>
       <c r="C9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D9" s="5">
         <v>112</v>
@@ -1291,7 +1288,7 @@
       <c r="E9" s="5">
         <v>52</v>
       </c>
-      <c r="F9" s="14">
+      <c r="F9" s="13">
         <f t="shared" si="0"/>
         <v>164</v>
       </c>
@@ -1310,27 +1307,25 @@
       <c r="K9" s="2">
         <v>0.71</v>
       </c>
-      <c r="L9" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="M9" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2">
+        <f t="shared" si="1"/>
+        <v>0.17232594379037389</v>
+      </c>
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
       <c r="R9" s="2"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B10">
         <v>2010</v>
       </c>
       <c r="C10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D10" s="5">
         <v>58</v>
@@ -1356,26 +1351,25 @@
       <c r="K10" s="2">
         <v>0.05</v>
       </c>
-      <c r="L10" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="M10" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2">
+        <f t="shared" si="1"/>
+        <v>0.18913238364476101</v>
+      </c>
+      <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
       <c r="R10" s="2"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B11">
         <v>2010</v>
       </c>
       <c r="C11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D11" s="5">
         <v>58</v>
@@ -1401,24 +1395,23 @@
       <c r="K11" s="2">
         <v>-0.71</v>
       </c>
-      <c r="L11" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="M11" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="O11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2">
+        <f t="shared" si="1"/>
+        <v>0.1949624175512675</v>
+      </c>
       <c r="P11" s="2"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B12">
         <v>2010</v>
       </c>
       <c r="C12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D12" s="5">
         <v>58</v>
@@ -1444,14 +1437,12 @@
       <c r="K12" s="2">
         <v>0.9</v>
       </c>
-      <c r="L12" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="M12" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="N12" s="2"/>
-      <c r="O12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2">
+        <f t="shared" si="1"/>
+        <v>0.19843379061398483</v>
+      </c>
       <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
       <c r="R12" s="2"/>
@@ -1464,7 +1455,7 @@
         <v>1988</v>
       </c>
       <c r="C13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D13" s="5">
         <v>24</v>
@@ -1472,8 +1463,8 @@
       <c r="E13" s="5">
         <v>24</v>
       </c>
-      <c r="F13" s="14">
-        <f t="shared" ref="F13:F14" si="1">D13+E13</f>
+      <c r="F13" s="13">
+        <f t="shared" ref="F13:F14" si="4">D13+E13</f>
         <v>48</v>
       </c>
       <c r="G13" s="4">
@@ -1497,21 +1488,30 @@
       <c r="M13" s="2">
         <v>-0.39</v>
       </c>
-      <c r="N13" s="10"/>
-      <c r="O13" s="2"/>
-      <c r="P13" s="2"/>
-      <c r="Q13" s="10"/>
-      <c r="R13" s="10"/>
+      <c r="N13" s="2">
+        <f t="shared" si="1"/>
+        <v>0.28879058156387305</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="2"/>
+        <v>0.2888933626790342</v>
+      </c>
+      <c r="P13" s="2">
+        <f t="shared" si="3"/>
+        <v>0.29140643152362533</v>
+      </c>
+      <c r="Q13" s="9"/>
+      <c r="R13" s="9"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B14">
         <v>2008</v>
       </c>
       <c r="C14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D14" s="5">
         <v>40</v>
@@ -1519,8 +1519,8 @@
       <c r="E14" s="5">
         <v>40</v>
       </c>
-      <c r="F14" s="14">
-        <f t="shared" si="1"/>
+      <c r="F14" s="13">
+        <f t="shared" si="4"/>
         <v>80</v>
       </c>
       <c r="G14" s="4">
@@ -1538,22 +1538,23 @@
       <c r="K14" s="2">
         <v>0.32</v>
       </c>
-      <c r="L14" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="M14" s="2" t="s">
-        <v>41</v>
-      </c>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2">
+        <f t="shared" si="1"/>
+        <v>0.22503333086456326</v>
+      </c>
+      <c r="P14" s="2"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B15">
         <v>2005</v>
       </c>
       <c r="C15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D15" s="5">
         <v>186</v>
@@ -1565,17 +1566,13 @@
         <v>80</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>41</v>
-      </c>
+        <v>138</v>
+      </c>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
       <c r="K15">
         <v>0.95</v>
       </c>
@@ -1585,16 +1582,28 @@
       <c r="M15">
         <v>1.35</v>
       </c>
+      <c r="N15" s="2">
+        <f t="shared" si="1"/>
+        <v>0.10938796006166132</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="2"/>
+        <v>0.10556809961306483</v>
+      </c>
+      <c r="P15" s="2">
+        <f t="shared" si="3"/>
+        <v>0.11490119645258948</v>
+      </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B16">
         <v>2005</v>
       </c>
       <c r="C16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D16" s="5">
         <v>186</v>
@@ -1606,17 +1615,13 @@
         <v>106</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>41</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
       <c r="K16">
         <v>0.09</v>
       </c>
@@ -1626,21 +1631,30 @@
       <c r="M16">
         <v>0.93</v>
       </c>
-      <c r="N16" s="2"/>
-      <c r="O16" s="2"/>
-      <c r="P16" s="2"/>
+      <c r="N16" s="2">
+        <f t="shared" si="1"/>
+        <v>0.10374765187134216</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="2"/>
+        <v>0.10718539862042477</v>
+      </c>
+      <c r="P16" s="2">
+        <f t="shared" si="3"/>
+        <v>0.10915671382028232</v>
+      </c>
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B17">
         <v>2004</v>
       </c>
       <c r="C17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D17" s="5">
         <v>23</v>
@@ -1648,8 +1662,8 @@
       <c r="E17" s="5">
         <v>20</v>
       </c>
-      <c r="F17" s="14">
-        <f t="shared" ref="F17:F32" si="2">D17+E17</f>
+      <c r="F17" s="13">
+        <f t="shared" ref="F17:F32" si="5">D17+E17</f>
         <v>43</v>
       </c>
       <c r="G17" s="4">
@@ -1667,24 +1681,23 @@
       <c r="K17" s="2">
         <v>-0.03</v>
       </c>
-      <c r="L17" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="M17" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="O17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2">
+        <f t="shared" si="1"/>
+        <v>0.30575926148825694</v>
+      </c>
       <c r="P17" s="2"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B18">
         <v>2001</v>
       </c>
       <c r="C18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D18" s="5">
         <v>26</v>
@@ -1692,22 +1705,18 @@
       <c r="E18" s="5">
         <v>23</v>
       </c>
-      <c r="F18" s="14">
-        <f t="shared" si="2"/>
+      <c r="F18" s="13">
+        <f t="shared" si="5"/>
         <v>49</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>41</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
       <c r="K18" s="2">
         <v>0.03</v>
       </c>
@@ -1717,20 +1726,30 @@
       <c r="M18" s="2">
         <v>0.39</v>
       </c>
-      <c r="O18" s="2"/>
-      <c r="P18" s="2"/>
+      <c r="N18" s="2">
+        <f t="shared" si="1"/>
+        <v>0.28626732786780446</v>
+      </c>
+      <c r="O18">
+        <f t="shared" si="2"/>
+        <v>0.29140231559681423</v>
+      </c>
+      <c r="P18" s="2">
+        <f t="shared" si="3"/>
+        <v>0.28894954602392131</v>
+      </c>
       <c r="Q18" s="2"/>
       <c r="R18" s="2"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B19">
         <v>2008</v>
       </c>
       <c r="C19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D19" s="5">
         <v>12</v>
@@ -1738,8 +1757,8 @@
       <c r="E19" s="5">
         <v>9</v>
       </c>
-      <c r="F19" s="14">
-        <f t="shared" si="2"/>
+      <c r="F19" s="13">
+        <f t="shared" si="5"/>
         <v>21</v>
       </c>
       <c r="G19" s="4">
@@ -1757,27 +1776,25 @@
       <c r="K19" s="2">
         <v>-0.89</v>
       </c>
-      <c r="L19" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="M19" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="N19" s="2"/>
-      <c r="O19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2">
+        <f t="shared" si="1"/>
+        <v>0.46184842562681561</v>
+      </c>
       <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
       <c r="R19" s="2"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B20">
         <v>2001</v>
       </c>
       <c r="C20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D20" s="5">
         <v>30</v>
@@ -1785,8 +1802,8 @@
       <c r="E20" s="5">
         <v>30</v>
       </c>
-      <c r="F20" s="14">
-        <f t="shared" si="2"/>
+      <c r="F20" s="13">
+        <f t="shared" si="5"/>
         <v>60</v>
       </c>
       <c r="G20" s="4">
@@ -1804,13 +1821,12 @@
       <c r="K20" s="2">
         <v>0.61</v>
       </c>
-      <c r="L20" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="M20" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="O20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2">
+        <f t="shared" si="1"/>
+        <v>0.26413538195402753</v>
+      </c>
       <c r="P20" s="2"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.2">
@@ -1821,7 +1837,7 @@
         <v>2002</v>
       </c>
       <c r="C21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D21" s="5">
         <v>58</v>
@@ -1829,8 +1845,8 @@
       <c r="E21" s="5">
         <v>58</v>
       </c>
-      <c r="F21" s="14">
-        <f t="shared" si="2"/>
+      <c r="F21" s="13">
+        <f t="shared" si="5"/>
         <v>116</v>
       </c>
       <c r="G21" s="4">
@@ -1839,22 +1855,23 @@
       <c r="H21" s="4">
         <v>70.3</v>
       </c>
-      <c r="I21" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="J21" s="2" t="s">
-        <v>41</v>
-      </c>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
       <c r="K21" s="2">
         <v>-0.61</v>
       </c>
       <c r="L21" s="2">
         <v>-0.84</v>
       </c>
-      <c r="M21" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="O21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2">
+        <f t="shared" si="1"/>
+        <v>0.18996483340617148</v>
+      </c>
+      <c r="O21">
+        <f t="shared" si="2"/>
+        <v>0.19371148115440778</v>
+      </c>
       <c r="P21" s="2"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.2">
@@ -1865,7 +1882,7 @@
         <v>2009</v>
       </c>
       <c r="C22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D22" s="5">
         <v>22</v>
@@ -1873,8 +1890,8 @@
       <c r="E22" s="5">
         <v>22</v>
       </c>
-      <c r="F22" s="14">
-        <f t="shared" si="2"/>
+      <c r="F22" s="13">
+        <f t="shared" si="5"/>
         <v>44</v>
       </c>
       <c r="G22" s="4">
@@ -1898,20 +1915,30 @@
       <c r="M22" s="2">
         <v>-0.69</v>
       </c>
-      <c r="N22" s="2"/>
-      <c r="P22" s="2"/>
+      <c r="N22" s="2">
+        <f t="shared" si="1"/>
+        <v>0.30436409118028362</v>
+      </c>
+      <c r="O22">
+        <f t="shared" si="2"/>
+        <v>0.30152830411392256</v>
+      </c>
+      <c r="P22" s="2">
+        <f t="shared" si="3"/>
+        <v>0.31035353740825672</v>
+      </c>
       <c r="Q22" s="2"/>
       <c r="R22" s="2"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B23">
         <v>2006</v>
       </c>
       <c r="C23" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D23" s="5">
         <v>42</v>
@@ -1919,8 +1946,8 @@
       <c r="E23" s="5">
         <v>45</v>
       </c>
-      <c r="F23" s="14">
-        <f t="shared" si="2"/>
+      <c r="F23" s="13">
+        <f t="shared" si="5"/>
         <v>87</v>
       </c>
       <c r="G23" s="4">
@@ -1938,26 +1965,25 @@
       <c r="K23" s="2">
         <v>-0.13</v>
       </c>
-      <c r="L23" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="M23" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="N23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2">
+        <f t="shared" si="1"/>
+        <v>0.21477633125772411</v>
+      </c>
       <c r="P23" s="2"/>
       <c r="Q23" s="2"/>
       <c r="R23" s="2"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B24">
         <v>2006</v>
       </c>
       <c r="C24" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D24" s="5">
         <v>50</v>
@@ -1965,8 +1991,8 @@
       <c r="E24" s="5">
         <v>53</v>
       </c>
-      <c r="F24" s="14">
-        <f t="shared" si="2"/>
+      <c r="F24" s="13">
+        <f t="shared" si="5"/>
         <v>103</v>
       </c>
       <c r="G24" s="4">
@@ -1975,36 +2001,30 @@
       <c r="H24" s="4">
         <v>71</v>
       </c>
-      <c r="I24" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="J24" s="2" t="s">
-        <v>41</v>
-      </c>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
       <c r="K24" s="2">
         <v>-0.03</v>
       </c>
-      <c r="L24" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="M24" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="N24" s="2"/>
-      <c r="O24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2">
+        <f t="shared" si="1"/>
+        <v>0.19716057785556604</v>
+      </c>
       <c r="P24" s="2"/>
       <c r="Q24" s="2"/>
       <c r="R24" s="2"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B25">
         <v>2011</v>
       </c>
       <c r="C25" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D25" s="5">
         <v>40</v>
@@ -2012,8 +2032,8 @@
       <c r="E25" s="5">
         <v>44</v>
       </c>
-      <c r="F25" s="14">
-        <f t="shared" si="2"/>
+      <c r="F25" s="13">
+        <f t="shared" si="5"/>
         <v>84</v>
       </c>
       <c r="G25" s="4">
@@ -2031,24 +2051,23 @@
       <c r="K25" s="2">
         <v>-0.23</v>
       </c>
-      <c r="L25" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="M25" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="O25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2">
+        <f t="shared" si="1"/>
+        <v>0.21918520406189301</v>
+      </c>
       <c r="P25" s="2"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B26">
         <v>2005</v>
       </c>
       <c r="C26" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D26" s="5">
         <v>192</v>
@@ -2056,8 +2075,8 @@
       <c r="E26" s="5">
         <v>192</v>
       </c>
-      <c r="F26" s="14">
-        <f t="shared" si="2"/>
+      <c r="F26" s="13">
+        <f t="shared" si="5"/>
         <v>384</v>
       </c>
       <c r="G26" s="4">
@@ -2081,21 +2100,30 @@
       <c r="M26" s="2">
         <v>0.1</v>
       </c>
-      <c r="N26" s="2"/>
-      <c r="O26" s="2"/>
-      <c r="P26" s="2"/>
+      <c r="N26" s="2">
+        <f t="shared" si="1"/>
+        <v>0.10207801856913172</v>
+      </c>
+      <c r="O26">
+        <f t="shared" si="2"/>
+        <v>0.10206207261596575</v>
+      </c>
+      <c r="P26" s="2">
+        <f t="shared" si="3"/>
+        <v>0.10212584148980119</v>
+      </c>
       <c r="Q26" s="2"/>
       <c r="R26" s="2"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B27">
         <v>2010</v>
       </c>
       <c r="C27" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D27" s="5">
         <v>35</v>
@@ -2103,8 +2131,8 @@
       <c r="E27" s="5">
         <v>42</v>
       </c>
-      <c r="F27" s="14">
-        <f t="shared" si="2"/>
+      <c r="F27" s="13">
+        <f t="shared" si="5"/>
         <v>77</v>
       </c>
       <c r="G27" s="4">
@@ -2122,27 +2150,25 @@
       <c r="K27" s="2">
         <v>0.5</v>
       </c>
-      <c r="L27" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="M27" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="N27" s="2"/>
-      <c r="O27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2">
+        <f t="shared" si="1"/>
+        <v>0.23238831512003569</v>
+      </c>
       <c r="P27" s="2"/>
       <c r="Q27" s="2"/>
       <c r="R27" s="2"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B28">
         <v>2011</v>
       </c>
       <c r="C28" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D28" s="5">
         <v>49</v>
@@ -2150,8 +2176,8 @@
       <c r="E28" s="5">
         <v>59</v>
       </c>
-      <c r="F28" s="14">
-        <f t="shared" si="2"/>
+      <c r="F28" s="13">
+        <f t="shared" si="5"/>
         <v>108</v>
       </c>
       <c r="G28" s="4">
@@ -2160,23 +2186,17 @@
       <c r="H28" s="4">
         <v>70.599999999999994</v>
       </c>
-      <c r="I28" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="J28" s="2" t="s">
-        <v>41</v>
-      </c>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
       <c r="K28" s="2">
         <v>0.43</v>
       </c>
-      <c r="L28" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="M28" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="N28" s="2"/>
-      <c r="O28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2">
+        <f t="shared" si="1"/>
+        <v>0.19548231205456293</v>
+      </c>
       <c r="P28" s="2"/>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.2">
@@ -2187,7 +2207,7 @@
         <v>2010</v>
       </c>
       <c r="C29" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D29" s="5">
         <v>51</v>
@@ -2195,8 +2215,8 @@
       <c r="E29" s="5">
         <v>24</v>
       </c>
-      <c r="F29" s="14">
-        <f t="shared" si="2"/>
+      <c r="F29" s="13">
+        <f t="shared" si="5"/>
         <v>75</v>
       </c>
       <c r="G29" s="4">
@@ -2211,28 +2231,27 @@
       <c r="J29" s="2">
         <v>12.2</v>
       </c>
-      <c r="K29" s="2" t="s">
-        <v>41</v>
-      </c>
+      <c r="K29" s="2"/>
       <c r="L29" s="2">
         <v>0.05</v>
       </c>
-      <c r="M29" s="2" t="s">
-        <v>41</v>
-      </c>
+      <c r="M29" s="2"/>
       <c r="N29" s="2"/>
-      <c r="O29" s="2"/>
+      <c r="O29">
+        <f t="shared" si="2"/>
+        <v>0.24757054847171994</v>
+      </c>
       <c r="P29" s="2"/>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B30">
         <v>2010</v>
       </c>
       <c r="C30" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D30" s="5">
         <v>661</v>
@@ -2240,8 +2259,8 @@
       <c r="E30" s="5">
         <v>168</v>
       </c>
-      <c r="F30" s="14">
-        <f t="shared" si="2"/>
+      <c r="F30" s="13">
+        <f t="shared" si="5"/>
         <v>829</v>
       </c>
       <c r="G30" s="4">
@@ -2250,33 +2269,34 @@
       <c r="H30" s="4">
         <v>72.5</v>
       </c>
-      <c r="I30" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="J30" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="K30" s="2" t="s">
-        <v>41</v>
-      </c>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
       <c r="L30" s="2">
         <v>0.06</v>
       </c>
       <c r="M30" s="2">
         <v>-3.43</v>
       </c>
-      <c r="O30" s="2"/>
-      <c r="P30" s="2"/>
+      <c r="N30" s="2"/>
+      <c r="O30">
+        <f t="shared" si="2"/>
+        <v>8.6414186029710266E-2</v>
+      </c>
+      <c r="P30" s="2">
+        <f t="shared" si="3"/>
+        <v>0.12066929442047349</v>
+      </c>
     </row>
     <row r="31" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B31">
         <v>2010</v>
       </c>
       <c r="C31" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D31" s="5">
         <v>358</v>
@@ -2284,22 +2304,18 @@
       <c r="E31" s="5">
         <v>61</v>
       </c>
-      <c r="F31" s="14">
-        <f t="shared" si="2"/>
+      <c r="F31" s="13">
+        <f t="shared" si="5"/>
         <v>419</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="I31" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="J31" s="2" t="s">
-        <v>41</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
       <c r="K31" s="2">
         <v>-0.24</v>
       </c>
@@ -2309,21 +2325,30 @@
       <c r="M31" s="2">
         <v>-0.1</v>
       </c>
-      <c r="N31" s="2"/>
-      <c r="O31" s="2"/>
-      <c r="P31" s="2"/>
+      <c r="N31" s="2">
+        <f t="shared" si="1"/>
+        <v>0.13876409404405923</v>
+      </c>
+      <c r="O31">
+        <f t="shared" si="2"/>
+        <v>0.13910465077583697</v>
+      </c>
+      <c r="P31" s="2">
+        <f t="shared" si="3"/>
+        <v>0.13855927210605806</v>
+      </c>
       <c r="Q31" s="2"/>
       <c r="R31" s="2"/>
     </row>
     <row r="32" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B32">
         <v>2005</v>
       </c>
       <c r="C32" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D32" s="5">
         <v>87</v>
@@ -2331,8 +2356,8 @@
       <c r="E32" s="5">
         <v>63</v>
       </c>
-      <c r="F32" s="14">
-        <f t="shared" si="2"/>
+      <c r="F32" s="13">
+        <f t="shared" si="5"/>
         <v>150</v>
       </c>
       <c r="G32" s="4">
@@ -2350,26 +2375,26 @@
       <c r="K32" s="2">
         <v>0.1</v>
       </c>
-      <c r="L32" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="M32" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="O32" s="2"/>
+      <c r="L32" s="2"/>
+      <c r="M32" s="2"/>
+      <c r="N32" s="2">
+        <f t="shared" si="1"/>
+        <v>0.16553127221136321</v>
+      </c>
+      <c r="O32"/>
       <c r="P32" s="2"/>
       <c r="Q32" s="2"/>
       <c r="R32" s="2"/>
     </row>
-    <row r="33" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B33">
         <v>2008</v>
       </c>
       <c r="C33" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D33" s="5">
         <v>33</v>
@@ -2377,7 +2402,7 @@
       <c r="E33" s="5">
         <v>52</v>
       </c>
-      <c r="F33" s="11">
+      <c r="F33" s="10">
         <v>85</v>
       </c>
       <c r="G33" s="4">
@@ -2395,22 +2420,24 @@
       <c r="K33" s="2">
         <v>0.76</v>
       </c>
-      <c r="L33" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="M33" s="12" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L33" s="11"/>
+      <c r="M33" s="11"/>
+      <c r="N33" s="2">
+        <f t="shared" si="1"/>
+        <v>0.230068352001363</v>
+      </c>
+      <c r="O33"/>
+      <c r="P33" s="2"/>
+    </row>
+    <row r="34" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B34">
         <v>2008</v>
       </c>
-      <c r="C34" s="11" t="s">
-        <v>72</v>
+      <c r="C34" s="10" t="s">
+        <v>71</v>
       </c>
       <c r="D34" s="5">
         <v>33</v>
@@ -2418,7 +2445,7 @@
       <c r="E34" s="5">
         <v>52</v>
       </c>
-      <c r="F34" s="11">
+      <c r="F34" s="10">
         <v>85</v>
       </c>
       <c r="G34" s="4">
@@ -2433,154 +2460,155 @@
       <c r="J34" s="2">
         <v>10.4</v>
       </c>
-      <c r="K34" s="13">
+      <c r="K34" s="12">
         <v>0.19</v>
       </c>
-      <c r="L34" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="M34" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="O34" s="9"/>
-    </row>
-    <row r="35" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="36" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="38" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="11"/>
-      <c r="B38" s="11"/>
-      <c r="C38" s="11"/>
-      <c r="D38" s="11"/>
-      <c r="E38" s="11"/>
-      <c r="F38" s="11"/>
-      <c r="G38" s="11"/>
-      <c r="H38" s="11"/>
-      <c r="I38" s="11"/>
-      <c r="J38" s="11"/>
-      <c r="K38" s="11"/>
-      <c r="L38" s="11"/>
-      <c r="M38" s="11"/>
-    </row>
-    <row r="39" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="11"/>
-      <c r="B39" s="11"/>
-      <c r="C39" s="11"/>
-      <c r="D39" s="11"/>
-      <c r="E39" s="11"/>
-      <c r="F39" s="11"/>
-      <c r="G39" s="11"/>
-      <c r="H39" s="11"/>
-      <c r="I39" s="11"/>
-      <c r="J39" s="11"/>
-      <c r="K39" s="11"/>
-      <c r="L39" s="11"/>
-      <c r="M39" s="11"/>
-    </row>
-    <row r="40" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="11"/>
-      <c r="B40" s="11"/>
-      <c r="C40" s="11"/>
-      <c r="D40" s="11"/>
-      <c r="E40" s="11"/>
-      <c r="F40" s="11"/>
-      <c r="G40" s="11"/>
-      <c r="H40" s="11"/>
-      <c r="I40" s="11"/>
-      <c r="J40" s="11"/>
-      <c r="K40" s="11"/>
-      <c r="L40" s="11"/>
-      <c r="M40" s="11"/>
-    </row>
-    <row r="41" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="11"/>
-      <c r="B41" s="11"/>
-      <c r="C41" s="11"/>
-      <c r="D41" s="11"/>
-      <c r="E41" s="11"/>
-      <c r="F41" s="11"/>
-      <c r="G41" s="11"/>
-      <c r="H41" s="11"/>
-      <c r="I41" s="11"/>
-      <c r="J41" s="11"/>
-      <c r="K41" s="11"/>
-      <c r="L41" s="11"/>
-      <c r="M41" s="11"/>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A42" s="11"/>
-      <c r="B42" s="11"/>
-      <c r="C42" s="11"/>
-      <c r="D42" s="11"/>
-      <c r="E42" s="11"/>
-      <c r="F42" s="11"/>
-      <c r="G42" s="11"/>
-      <c r="H42" s="11"/>
-      <c r="I42" s="11"/>
-      <c r="J42" s="11"/>
-      <c r="K42" s="11"/>
-      <c r="L42" s="11"/>
-      <c r="M42" s="11"/>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A43" s="11"/>
-      <c r="B43" s="11"/>
-      <c r="C43" s="11"/>
-      <c r="D43" s="11"/>
-      <c r="E43" s="11"/>
-      <c r="F43" s="11"/>
-      <c r="G43" s="11"/>
-      <c r="H43" s="11"/>
-      <c r="I43" s="11"/>
-      <c r="J43" s="11"/>
-      <c r="K43" s="11"/>
-      <c r="L43" s="11"/>
-      <c r="M43" s="11"/>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A44" s="11"/>
-      <c r="B44" s="11"/>
-      <c r="C44" s="11"/>
-      <c r="D44" s="11"/>
-      <c r="E44" s="11"/>
-      <c r="F44" s="11"/>
-      <c r="G44" s="11"/>
-      <c r="H44" s="11"/>
-      <c r="I44" s="11"/>
-      <c r="J44" s="11"/>
-      <c r="K44" s="11"/>
-      <c r="L44" s="11"/>
-      <c r="M44" s="11"/>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A45" s="11"/>
-      <c r="B45" s="11"/>
-      <c r="C45" s="11"/>
-      <c r="D45" s="11"/>
-      <c r="E45" s="11"/>
-      <c r="F45" s="11"/>
-      <c r="G45" s="11"/>
-      <c r="H45" s="11"/>
-      <c r="I45" s="11"/>
-      <c r="J45" s="11"/>
-      <c r="K45" s="11"/>
-      <c r="L45" s="11"/>
-      <c r="M45" s="11"/>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A46" s="11"/>
-      <c r="B46" s="11"/>
-      <c r="C46" s="11"/>
-      <c r="D46" s="11"/>
-      <c r="E46" s="11"/>
-      <c r="F46" s="11"/>
-      <c r="G46" s="11"/>
-      <c r="H46" s="11"/>
-      <c r="I46" s="11"/>
-      <c r="J46" s="11"/>
-      <c r="K46" s="11"/>
-      <c r="L46" s="11"/>
-      <c r="M46" s="11"/>
+      <c r="L34" s="11"/>
+      <c r="M34" s="11"/>
+      <c r="N34" s="2">
+        <f t="shared" si="1"/>
+        <v>0.22303845514838019</v>
+      </c>
+      <c r="O34"/>
+      <c r="P34" s="2"/>
+    </row>
+    <row r="35" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="10"/>
+      <c r="B38" s="10"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="10"/>
+      <c r="F38" s="10"/>
+      <c r="G38" s="10"/>
+      <c r="H38" s="10"/>
+      <c r="I38" s="10"/>
+      <c r="J38" s="10"/>
+      <c r="K38" s="10"/>
+      <c r="L38" s="10"/>
+      <c r="M38" s="10"/>
+    </row>
+    <row r="39" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="10"/>
+      <c r="B39" s="10"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="10"/>
+      <c r="H39" s="10"/>
+      <c r="I39" s="10"/>
+      <c r="J39" s="10"/>
+      <c r="K39" s="10"/>
+      <c r="L39" s="10"/>
+      <c r="M39" s="10"/>
+    </row>
+    <row r="40" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="10"/>
+      <c r="B40" s="10"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="10"/>
+      <c r="H40" s="10"/>
+      <c r="I40" s="10"/>
+      <c r="J40" s="10"/>
+      <c r="K40" s="10"/>
+      <c r="L40" s="10"/>
+      <c r="M40" s="10"/>
+    </row>
+    <row r="41" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="10"/>
+      <c r="B41" s="10"/>
+      <c r="C41" s="10"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="10"/>
+      <c r="H41" s="10"/>
+      <c r="I41" s="10"/>
+      <c r="J41" s="10"/>
+      <c r="K41" s="10"/>
+      <c r="L41" s="10"/>
+      <c r="M41" s="10"/>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A42" s="10"/>
+      <c r="B42" s="10"/>
+      <c r="C42" s="10"/>
+      <c r="D42" s="10"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="10"/>
+      <c r="G42" s="10"/>
+      <c r="H42" s="10"/>
+      <c r="I42" s="10"/>
+      <c r="J42" s="10"/>
+      <c r="K42" s="10"/>
+      <c r="L42" s="10"/>
+      <c r="M42" s="10"/>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A43" s="10"/>
+      <c r="B43" s="10"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="10"/>
+      <c r="G43" s="10"/>
+      <c r="H43" s="10"/>
+      <c r="I43" s="10"/>
+      <c r="J43" s="10"/>
+      <c r="K43" s="10"/>
+      <c r="L43" s="10"/>
+      <c r="M43" s="10"/>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A44" s="10"/>
+      <c r="B44" s="10"/>
+      <c r="C44" s="10"/>
+      <c r="D44" s="10"/>
+      <c r="E44" s="10"/>
+      <c r="F44" s="10"/>
+      <c r="G44" s="10"/>
+      <c r="H44" s="10"/>
+      <c r="I44" s="10"/>
+      <c r="J44" s="10"/>
+      <c r="K44" s="10"/>
+      <c r="L44" s="10"/>
+      <c r="M44" s="10"/>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A45" s="10"/>
+      <c r="B45" s="10"/>
+      <c r="C45" s="10"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="10"/>
+      <c r="F45" s="10"/>
+      <c r="G45" s="10"/>
+      <c r="H45" s="10"/>
+      <c r="I45" s="10"/>
+      <c r="J45" s="10"/>
+      <c r="K45" s="10"/>
+      <c r="L45" s="10"/>
+      <c r="M45" s="10"/>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A46" s="10"/>
+      <c r="B46" s="10"/>
+      <c r="C46" s="10"/>
+      <c r="D46" s="10"/>
+      <c r="E46" s="10"/>
+      <c r="F46" s="10"/>
+      <c r="G46" s="10"/>
+      <c r="H46" s="10"/>
+      <c r="I46" s="10"/>
+      <c r="J46" s="10"/>
+      <c r="K46" s="10"/>
+      <c r="L46" s="10"/>
+      <c r="M46" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -2591,20 +2619,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C4FF05C-65B7-4CF6-8702-24FB92544144}">
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N21" sqref="N21"/>
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>4</v>
@@ -2624,8 +2652,14 @@
       <c r="H1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I1" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -2650,8 +2684,16 @@
       <c r="H2" s="2">
         <v>0.04</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I2">
+        <f>SQRT((C2+D2)/(C2*D2)+G2^2/(2*(C2+D2)))</f>
+        <v>0.18475372863020592</v>
+      </c>
+      <c r="J2">
+        <f>SQRT((C2+D2)/(C2*D2)+H2^2/(2*(C2+D2)))</f>
+        <v>0.18367602298404209</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -2676,8 +2718,16 @@
       <c r="H3" s="2">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I3">
+        <f t="shared" ref="I3:I36" si="0">SQRT((C3+D3)/(C3*D3)+G3^2/(2*(C3+D3)))</f>
+        <v>0.18366801638489966</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J36" si="1">SQRT((C3+D3)/(C3*D3)+H3^2/(2*(C3+D3)))</f>
+        <v>0.18366801638489966</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -2702,8 +2752,16 @@
       <c r="H4" s="2">
         <v>-0.21</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I4">
+        <f t="shared" si="0"/>
+        <v>0.2888933626790342</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="1"/>
+        <v>0.2894697019263559</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -2728,8 +2786,16 @@
       <c r="H5" s="2">
         <v>-1.26</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>0.13746026192572441</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="1"/>
+        <v>0.14616881886602476</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -2754,8 +2820,16 @@
       <c r="H6" s="2">
         <v>1.33</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>0.19776582301984583</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="1"/>
+        <v>0.21466186662081385</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -2780,8 +2854,16 @@
       <c r="H7" s="2">
         <v>0.93</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I7">
+        <f t="shared" si="0"/>
+        <v>0.20364716990746703</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="1"/>
+        <v>0.20448854744883843</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -2806,8 +2888,16 @@
       <c r="H8" s="2">
         <v>1.52</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>0.23113307854999898</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="1"/>
+        <v>0.25385034961567415</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -2832,8 +2922,16 @@
       <c r="H9" s="2">
         <v>0.55000000000000004</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>0.22891592343041584</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="1"/>
+        <v>0.22779513822731162</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -2858,8 +2956,16 @@
       <c r="H10" s="2">
         <v>0.38</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>0.29140231559681423</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="1"/>
+        <v>0.28881355355810223</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -2881,11 +2987,13 @@
       <c r="G11" s="2">
         <v>-0.8</v>
       </c>
-      <c r="H11" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H11" s="2"/>
+      <c r="I11">
+        <f t="shared" si="0"/>
+        <v>0.23841582427170788</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -2907,11 +3015,13 @@
       <c r="G12" s="2">
         <v>-0.86</v>
       </c>
-      <c r="H12" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H12" s="2"/>
+      <c r="I12">
+        <f t="shared" si="0"/>
+        <v>0.21335123622796281</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -2930,14 +3040,16 @@
       <c r="F13" t="s">
         <v>39</v>
       </c>
-      <c r="G13" s="2" t="s">
-        <v>41</v>
-      </c>
+      <c r="G13" s="2"/>
       <c r="H13" s="2">
         <v>1.65</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J13">
+        <f t="shared" si="1"/>
+        <v>0.3661027861134083</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -2962,8 +3074,16 @@
       <c r="H14" s="2">
         <v>0.36</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I14">
+        <f t="shared" si="0"/>
+        <v>0.17133960242943319</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="1"/>
+        <v>0.17250661797747513</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -2988,8 +3108,16 @@
       <c r="H15" s="2">
         <v>-0.28999999999999998</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I15">
+        <f t="shared" si="0"/>
+        <v>0.18969235528922196</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="1"/>
+        <v>0.18666884748315574</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -3014,8 +3142,16 @@
       <c r="H16" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I16">
+        <f t="shared" si="0"/>
+        <v>0.19280260586305933</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="1"/>
+        <v>0.18569533817705186</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -3040,8 +3176,16 @@
       <c r="H17" s="2">
         <v>0.33</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I17">
+        <f t="shared" si="0"/>
+        <v>0.11568464641269635</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="1"/>
+        <v>0.11620270835411668</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -3066,8 +3210,16 @@
       <c r="H18" s="2">
         <v>-0.7</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I18">
+        <f t="shared" si="0"/>
+        <v>0.30152830411392256</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="1"/>
+        <v>0.31060790834631485</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -3092,8 +3244,16 @@
       <c r="H19" s="2">
         <v>-1.06</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I19">
+        <f t="shared" si="0"/>
+        <v>0.26760511953249322</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="1"/>
+        <v>0.26697963405473457</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>35</v>
       </c>
@@ -3118,8 +3278,16 @@
       <c r="H20" s="2">
         <v>-0.24</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I20">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="1"/>
+        <v>0.25089838580588758</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>36</v>
       </c>
@@ -3144,8 +3312,16 @@
       <c r="H21" s="2">
         <v>0.48</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I21">
+        <f t="shared" si="0"/>
+        <v>0.26760511953249322</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="1"/>
+        <v>0.25357444666211931</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -3167,11 +3343,13 @@
       <c r="G22" s="2">
         <v>0.05</v>
       </c>
-      <c r="H22" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H22" s="2"/>
+      <c r="I22">
+        <f t="shared" si="0"/>
+        <v>0.24757054847171994</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -3193,11 +3371,13 @@
       <c r="G23" s="2">
         <v>-0.3</v>
       </c>
-      <c r="H23" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H23" s="2"/>
+      <c r="I23">
+        <f t="shared" si="0"/>
+        <v>0.2901149197588202</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -3222,8 +3402,16 @@
       <c r="H24" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I24">
+        <f t="shared" si="0"/>
+        <v>0.17165286447465111</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="1"/>
+        <v>0.17155109854432499</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -3248,8 +3436,16 @@
       <c r="H25" s="2">
         <v>0.04</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I25">
+        <f t="shared" si="0"/>
+        <v>0.17173958569333295</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="1"/>
+        <v>0.1715157341436159</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -3274,8 +3470,16 @@
       <c r="H26" s="2">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I26">
+        <f t="shared" si="0"/>
+        <v>0.18259244234085922</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="1"/>
+        <v>0.18888378261071895</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -3300,8 +3504,16 @@
       <c r="H27" s="2">
         <v>-0.04</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I27">
+        <f t="shared" si="0"/>
+        <v>0.18264720090929398</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="1"/>
+        <v>0.18259244234085922</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -3326,8 +3538,16 @@
       <c r="H28" s="2">
         <v>-0.19</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I28">
+        <f t="shared" si="0"/>
+        <v>0.24117918572405303</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="1"/>
+        <v>0.23968187171022609</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -3349,11 +3569,13 @@
       <c r="G29" s="2">
         <v>-1.1299999999999999</v>
       </c>
-      <c r="H29" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H29" s="2"/>
+      <c r="I29">
+        <f t="shared" si="0"/>
+        <v>0.20216920487799878</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -3375,11 +3597,13 @@
       <c r="G30" s="2">
         <v>-0.89</v>
       </c>
-      <c r="H30" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H30" s="2"/>
+      <c r="I30">
+        <f t="shared" si="0"/>
+        <v>0.19743008231017442</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -3398,14 +3622,16 @@
       <c r="F31" t="s">
         <v>6</v>
       </c>
-      <c r="G31" s="2" t="s">
-        <v>41</v>
-      </c>
+      <c r="G31" s="2"/>
       <c r="H31" s="2">
         <v>-1.93</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J31">
+        <f t="shared" si="1"/>
+        <v>0.2280392653060917</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -3424,14 +3650,16 @@
       <c r="F32" t="s">
         <v>40</v>
       </c>
-      <c r="G32" s="2" t="s">
-        <v>41</v>
-      </c>
+      <c r="G32" s="2"/>
       <c r="H32" s="2">
         <v>-1.59</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J32">
+        <f t="shared" si="1"/>
+        <v>0.21701840587506674</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -3456,8 +3684,16 @@
       <c r="H33" s="2">
         <v>-0.1</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I33">
+        <f t="shared" si="0"/>
+        <v>0.14131409792796853</v>
+      </c>
+      <c r="J33">
+        <f t="shared" si="1"/>
+        <v>0.13855927210605806</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -3482,8 +3718,16 @@
       <c r="H34" s="2">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I34">
+        <f t="shared" si="0"/>
+        <v>0.25892901349699249</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="1"/>
+        <v>0.25639839248690693</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -3508,8 +3752,16 @@
       <c r="H35" s="2">
         <v>-0.44</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I35">
+        <f t="shared" si="0"/>
+        <v>0.26846630416153161</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="1"/>
+        <v>0.26144627836355216</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -3533,6 +3785,14 @@
       </c>
       <c r="H36" s="2">
         <v>-0.22</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="0"/>
+        <v>0.24447009019509933</v>
+      </c>
+      <c r="J36">
+        <f t="shared" si="1"/>
+        <v>0.2242821883253327</v>
       </c>
     </row>
   </sheetData>
@@ -3546,7 +3806,7 @@
   <dimension ref="A1:G45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+      <selection activeCell="K45" sqref="K45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3558,27 +3818,27 @@
   <sheetData>
     <row r="1" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="D1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>91</v>
-      </c>
       <c r="F1" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>135</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="2" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C2">
         <v>1994</v>
@@ -3598,7 +3858,7 @@
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C3">
         <v>2012</v>
@@ -3618,7 +3878,7 @@
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C4">
         <v>2013</v>
@@ -3638,7 +3898,7 @@
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C5">
         <v>2018</v>
@@ -3658,7 +3918,7 @@
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C6">
         <v>2011</v>
@@ -3678,7 +3938,7 @@
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C7">
         <v>2018</v>
@@ -3698,7 +3958,7 @@
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C8">
         <v>2015</v>
@@ -3718,7 +3978,7 @@
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C9">
         <v>2016</v>
@@ -3738,7 +3998,7 @@
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C10">
         <v>2015</v>
@@ -3758,7 +4018,7 @@
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C11">
         <v>2013</v>
@@ -3778,7 +4038,7 @@
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C12">
         <v>2018</v>
@@ -3798,10 +4058,10 @@
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D13" s="6">
         <v>74</v>
@@ -3818,7 +4078,7 @@
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C14">
         <v>2009</v>
@@ -3838,7 +4098,7 @@
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C15">
         <v>2014</v>
@@ -3858,7 +4118,7 @@
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C16">
         <v>2018</v>
@@ -3878,7 +4138,7 @@
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C17">
         <v>2018</v>
@@ -3898,7 +4158,7 @@
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C18">
         <v>2012</v>
@@ -3918,7 +4178,7 @@
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C19">
         <v>2016</v>
@@ -3938,7 +4198,7 @@
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C20">
         <v>2018</v>
@@ -3958,7 +4218,7 @@
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C21">
         <v>2016</v>
@@ -3978,10 +4238,10 @@
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D22" s="6">
         <v>2630</v>
@@ -3998,7 +4258,7 @@
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C23">
         <v>2018</v>
@@ -4018,7 +4278,7 @@
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C24">
         <v>2018</v>
@@ -4038,7 +4298,7 @@
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C25">
         <v>2018</v>
@@ -4058,7 +4318,7 @@
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C26">
         <v>2019</v>
@@ -4078,7 +4338,7 @@
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C27">
         <v>2017</v>
@@ -4098,7 +4358,7 @@
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C28">
         <v>2011</v>
@@ -4118,7 +4378,7 @@
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C29">
         <v>2013</v>
@@ -4138,7 +4398,7 @@
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C30">
         <v>2016</v>
@@ -4158,10 +4418,10 @@
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C31" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D31" s="6">
         <v>619</v>
@@ -4178,7 +4438,7 @@
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C32">
         <v>2010</v>
@@ -4198,7 +4458,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C33">
         <v>2016</v>
@@ -4218,7 +4478,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C34">
         <v>2009</v>
@@ -4238,7 +4498,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C35">
         <v>2009</v>
@@ -4258,7 +4518,7 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C36">
         <v>2018</v>
@@ -4278,7 +4538,7 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C37">
         <v>2018</v>
@@ -4298,7 +4558,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C38">
         <v>2018</v>
@@ -4318,7 +4578,7 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C39">
         <v>2012</v>
@@ -4338,7 +4598,7 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C40">
         <v>2002</v>
@@ -4358,7 +4618,7 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C41">
         <v>2011</v>
@@ -4378,7 +4638,7 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C42">
         <v>2015</v>
@@ -4399,7 +4659,7 @@
     <row r="43" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="44" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D44" s="7">
         <f>SUBTOTAL(9,D2:D42)</f>
@@ -4414,7 +4674,7 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -4437,18 +4697,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8D7E26E-2B75-4FC8-A793-1D7462D1F2E7}">
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>4</v>
@@ -4457,30 +4717,30 @@
         <v>5</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="I1" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="14" t="s">
         <v>142</v>
-      </c>
-      <c r="K1" s="15" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B2">
         <v>2013</v>
@@ -4512,7 +4772,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B3">
         <v>2018</v>
@@ -4544,7 +4804,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B4">
         <v>2013</v>
@@ -4576,7 +4836,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B5">
         <v>2014</v>
@@ -4605,7 +4865,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B6">
         <v>2017</v>
@@ -4622,7 +4882,7 @@
       <c r="G6">
         <v>73.63</v>
       </c>
-      <c r="H6" s="16">
+      <c r="H6" s="15">
         <v>2.9002292479318501E-2</v>
       </c>
       <c r="I6">
@@ -4637,7 +4897,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B7">
         <v>2019</v>
@@ -4669,7 +4929,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B8">
         <v>2016</v>
@@ -4701,7 +4961,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B9">
         <v>2014</v>
@@ -4727,7 +4987,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B10">
         <v>2017</v>
@@ -4759,7 +5019,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B11">
         <v>2012</v>
@@ -4791,7 +5051,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B12">
         <v>2016</v>
@@ -4823,7 +5083,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B13">
         <v>2019</v>
@@ -4855,7 +5115,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B14">
         <v>2018</v>
@@ -4887,7 +5147,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B15">
         <v>2018</v>
@@ -4919,7 +5179,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B16">
         <v>2019</v>
@@ -4951,7 +5211,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B17">
         <v>2012</v>

</xml_diff>

<commit_message>
updated scripts and figures
Splitting risk into gain and loss
created an outcome folder to save the cma output
started some plotting
</commit_message>
<xml_diff>
--- a/data/cumulative_ma_data.xlsx
+++ b/data/cumulative_ma_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abagaini/Documents/PROJECTS/Cumul_MA/cumulative/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB850629-CC27-2F4D-9730-56950F7143B7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33950608-D42B-CE45-A322-1367AF0BC4AE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17060" xr2:uid="{D15F3EFF-771D-497D-BAA4-C31EA9079474}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17060" activeTab="1" xr2:uid="{D15F3EFF-771D-497D-BAA4-C31EA9079474}"/>
   </bookViews>
   <sheets>
     <sheet name="Mata_et_al(2011)" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="158">
   <si>
     <t>g_pos</t>
   </si>
@@ -502,21 +502,6 @@
   </si>
   <si>
     <t>Sze</t>
-  </si>
-  <si>
-    <t>se_pos</t>
-  </si>
-  <si>
-    <t>se_neg</t>
-  </si>
-  <si>
-    <t>se_all</t>
-  </si>
-  <si>
-    <t>se_gains</t>
-  </si>
-  <si>
-    <t>se_losses</t>
   </si>
 </sst>
 </file>
@@ -913,8 +898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38FBD286-E9F4-43DE-AE76-F152A62FC2EB}">
   <dimension ref="A1:R46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N1" sqref="N1:R1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -962,15 +947,6 @@
       <c r="M1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>162</v>
-      </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -1005,10 +981,7 @@
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
-      <c r="N2" s="2">
-        <f>SQRT((D2+E2)/(D2*E2)+K2^2/(2*(D2+E2)))</f>
-        <v>0.35363293115885008</v>
-      </c>
+      <c r="N2" s="2"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
@@ -1046,10 +1019,7 @@
       </c>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
-      <c r="N3" s="2">
-        <f t="shared" ref="N3:N34" si="1">SQRT((D3+E3)/(D3*E3)+K3^2/(2*(D3+E3)))</f>
-        <v>0.26503990991198634</v>
-      </c>
+      <c r="N3" s="2"/>
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
@@ -1091,18 +1061,8 @@
       <c r="M4" s="2">
         <v>0</v>
       </c>
-      <c r="N4" s="2">
-        <f t="shared" si="1"/>
-        <v>0.18407020237514718</v>
-      </c>
-      <c r="O4">
-        <f t="shared" ref="O4:O31" si="2">SQRT((D4+E4)/(D4*E4)+L4^2/(2*(D4+E4)))</f>
-        <v>0.18391491659265916</v>
-      </c>
-      <c r="P4" s="2">
-        <f t="shared" ref="P4:P31" si="3">SQRT((D4+E4)/(D4*E4)+M4^2/(2*(D4+E4)))</f>
-        <v>0.18365772167311323</v>
-      </c>
+      <c r="N4" s="2"/>
+      <c r="P4" s="2"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -1137,10 +1097,7 @@
       </c>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
-      <c r="N5" s="2">
-        <f t="shared" si="1"/>
-        <v>0.21718928853627611</v>
-      </c>
+      <c r="N5" s="2"/>
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
@@ -1178,10 +1135,7 @@
       </c>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
-      <c r="N6" s="2">
-        <f t="shared" si="1"/>
-        <v>0.31022572427185985</v>
-      </c>
+      <c r="N6" s="2"/>
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
       <c r="R6" s="2"/>
@@ -1223,10 +1177,7 @@
       </c>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
-      <c r="N7" s="2">
-        <f t="shared" si="1"/>
-        <v>0.16466557843681137</v>
-      </c>
+      <c r="N7" s="2"/>
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
@@ -1264,10 +1215,7 @@
       </c>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
-      <c r="N8" s="2">
-        <f t="shared" si="1"/>
-        <v>0.33752571918464391</v>
-      </c>
+      <c r="N8" s="2"/>
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
       <c r="R8" s="2"/>
@@ -1309,10 +1257,7 @@
       </c>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
-      <c r="N9" s="2">
-        <f t="shared" si="1"/>
-        <v>0.17232594379037389</v>
-      </c>
+      <c r="N9" s="2"/>
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
       <c r="R9" s="2"/>
@@ -1353,10 +1298,7 @@
       </c>
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
-      <c r="N10" s="2">
-        <f t="shared" si="1"/>
-        <v>0.18913238364476101</v>
-      </c>
+      <c r="N10" s="2"/>
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
       <c r="R10" s="2"/>
@@ -1397,10 +1339,7 @@
       </c>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
-      <c r="N11" s="2">
-        <f t="shared" si="1"/>
-        <v>0.1949624175512675</v>
-      </c>
+      <c r="N11" s="2"/>
       <c r="P11" s="2"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
@@ -1439,10 +1378,7 @@
       </c>
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
-      <c r="N12" s="2">
-        <f t="shared" si="1"/>
-        <v>0.19843379061398483</v>
-      </c>
+      <c r="N12" s="2"/>
       <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
       <c r="R12" s="2"/>
@@ -1464,7 +1400,7 @@
         <v>24</v>
       </c>
       <c r="F13" s="13">
-        <f t="shared" ref="F13:F14" si="4">D13+E13</f>
+        <f t="shared" ref="F13:F14" si="1">D13+E13</f>
         <v>48</v>
       </c>
       <c r="G13" s="4">
@@ -1488,18 +1424,8 @@
       <c r="M13" s="2">
         <v>-0.39</v>
       </c>
-      <c r="N13" s="2">
-        <f t="shared" si="1"/>
-        <v>0.28879058156387305</v>
-      </c>
-      <c r="O13">
-        <f t="shared" si="2"/>
-        <v>0.2888933626790342</v>
-      </c>
-      <c r="P13" s="2">
-        <f t="shared" si="3"/>
-        <v>0.29140643152362533</v>
-      </c>
+      <c r="N13" s="2"/>
+      <c r="P13" s="2"/>
       <c r="Q13" s="9"/>
       <c r="R13" s="9"/>
     </row>
@@ -1520,7 +1446,7 @@
         <v>40</v>
       </c>
       <c r="F14" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>80</v>
       </c>
       <c r="G14" s="4">
@@ -1540,10 +1466,7 @@
       </c>
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
-      <c r="N14" s="2">
-        <f t="shared" si="1"/>
-        <v>0.22503333086456326</v>
-      </c>
+      <c r="N14" s="2"/>
       <c r="P14" s="2"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
@@ -1582,18 +1505,8 @@
       <c r="M15">
         <v>1.35</v>
       </c>
-      <c r="N15" s="2">
-        <f t="shared" si="1"/>
-        <v>0.10938796006166132</v>
-      </c>
-      <c r="O15">
-        <f t="shared" si="2"/>
-        <v>0.10556809961306483</v>
-      </c>
-      <c r="P15" s="2">
-        <f t="shared" si="3"/>
-        <v>0.11490119645258948</v>
-      </c>
+      <c r="N15" s="2"/>
+      <c r="P15" s="2"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
@@ -1631,18 +1544,8 @@
       <c r="M16">
         <v>0.93</v>
       </c>
-      <c r="N16" s="2">
-        <f t="shared" si="1"/>
-        <v>0.10374765187134216</v>
-      </c>
-      <c r="O16">
-        <f t="shared" si="2"/>
-        <v>0.10718539862042477</v>
-      </c>
-      <c r="P16" s="2">
-        <f t="shared" si="3"/>
-        <v>0.10915671382028232</v>
-      </c>
+      <c r="N16" s="2"/>
+      <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
     </row>
@@ -1663,7 +1566,7 @@
         <v>20</v>
       </c>
       <c r="F17" s="13">
-        <f t="shared" ref="F17:F32" si="5">D17+E17</f>
+        <f t="shared" ref="F17:F32" si="2">D17+E17</f>
         <v>43</v>
       </c>
       <c r="G17" s="4">
@@ -1683,10 +1586,7 @@
       </c>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
-      <c r="N17" s="2">
-        <f t="shared" si="1"/>
-        <v>0.30575926148825694</v>
-      </c>
+      <c r="N17" s="2"/>
       <c r="P17" s="2"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.2">
@@ -1706,7 +1606,7 @@
         <v>23</v>
       </c>
       <c r="F18" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>49</v>
       </c>
       <c r="G18" s="4" t="s">
@@ -1726,18 +1626,8 @@
       <c r="M18" s="2">
         <v>0.39</v>
       </c>
-      <c r="N18" s="2">
-        <f t="shared" si="1"/>
-        <v>0.28626732786780446</v>
-      </c>
-      <c r="O18">
-        <f t="shared" si="2"/>
-        <v>0.29140231559681423</v>
-      </c>
-      <c r="P18" s="2">
-        <f t="shared" si="3"/>
-        <v>0.28894954602392131</v>
-      </c>
+      <c r="N18" s="2"/>
+      <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
       <c r="R18" s="2"/>
     </row>
@@ -1758,7 +1648,7 @@
         <v>9</v>
       </c>
       <c r="F19" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>21</v>
       </c>
       <c r="G19" s="4">
@@ -1778,10 +1668,7 @@
       </c>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
-      <c r="N19" s="2">
-        <f t="shared" si="1"/>
-        <v>0.46184842562681561</v>
-      </c>
+      <c r="N19" s="2"/>
       <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
       <c r="R19" s="2"/>
@@ -1803,7 +1690,7 @@
         <v>30</v>
       </c>
       <c r="F20" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>60</v>
       </c>
       <c r="G20" s="4">
@@ -1823,10 +1710,7 @@
       </c>
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
-      <c r="N20" s="2">
-        <f t="shared" si="1"/>
-        <v>0.26413538195402753</v>
-      </c>
+      <c r="N20" s="2"/>
       <c r="P20" s="2"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.2">
@@ -1846,7 +1730,7 @@
         <v>58</v>
       </c>
       <c r="F21" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>116</v>
       </c>
       <c r="G21" s="4">
@@ -1864,14 +1748,7 @@
         <v>-0.84</v>
       </c>
       <c r="M21" s="2"/>
-      <c r="N21" s="2">
-        <f t="shared" si="1"/>
-        <v>0.18996483340617148</v>
-      </c>
-      <c r="O21">
-        <f t="shared" si="2"/>
-        <v>0.19371148115440778</v>
-      </c>
+      <c r="N21" s="2"/>
       <c r="P21" s="2"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.2">
@@ -1891,7 +1768,7 @@
         <v>22</v>
       </c>
       <c r="F22" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>44</v>
       </c>
       <c r="G22" s="4">
@@ -1915,18 +1792,8 @@
       <c r="M22" s="2">
         <v>-0.69</v>
       </c>
-      <c r="N22" s="2">
-        <f t="shared" si="1"/>
-        <v>0.30436409118028362</v>
-      </c>
-      <c r="O22">
-        <f t="shared" si="2"/>
-        <v>0.30152830411392256</v>
-      </c>
-      <c r="P22" s="2">
-        <f t="shared" si="3"/>
-        <v>0.31035353740825672</v>
-      </c>
+      <c r="N22" s="2"/>
+      <c r="P22" s="2"/>
       <c r="Q22" s="2"/>
       <c r="R22" s="2"/>
     </row>
@@ -1947,7 +1814,7 @@
         <v>45</v>
       </c>
       <c r="F23" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>87</v>
       </c>
       <c r="G23" s="4">
@@ -1967,10 +1834,7 @@
       </c>
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
-      <c r="N23" s="2">
-        <f t="shared" si="1"/>
-        <v>0.21477633125772411</v>
-      </c>
+      <c r="N23" s="2"/>
       <c r="P23" s="2"/>
       <c r="Q23" s="2"/>
       <c r="R23" s="2"/>
@@ -1992,7 +1856,7 @@
         <v>53</v>
       </c>
       <c r="F24" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>103</v>
       </c>
       <c r="G24" s="4">
@@ -2008,10 +1872,7 @@
       </c>
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
-      <c r="N24" s="2">
-        <f t="shared" si="1"/>
-        <v>0.19716057785556604</v>
-      </c>
+      <c r="N24" s="2"/>
       <c r="P24" s="2"/>
       <c r="Q24" s="2"/>
       <c r="R24" s="2"/>
@@ -2033,7 +1894,7 @@
         <v>44</v>
       </c>
       <c r="F25" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>84</v>
       </c>
       <c r="G25" s="4">
@@ -2053,10 +1914,7 @@
       </c>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
-      <c r="N25" s="2">
-        <f t="shared" si="1"/>
-        <v>0.21918520406189301</v>
-      </c>
+      <c r="N25" s="2"/>
       <c r="P25" s="2"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.2">
@@ -2076,7 +1934,7 @@
         <v>192</v>
       </c>
       <c r="F26" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>384</v>
       </c>
       <c r="G26" s="4">
@@ -2100,18 +1958,8 @@
       <c r="M26" s="2">
         <v>0.1</v>
       </c>
-      <c r="N26" s="2">
-        <f t="shared" si="1"/>
-        <v>0.10207801856913172</v>
-      </c>
-      <c r="O26">
-        <f t="shared" si="2"/>
-        <v>0.10206207261596575</v>
-      </c>
-      <c r="P26" s="2">
-        <f t="shared" si="3"/>
-        <v>0.10212584148980119</v>
-      </c>
+      <c r="N26" s="2"/>
+      <c r="P26" s="2"/>
       <c r="Q26" s="2"/>
       <c r="R26" s="2"/>
     </row>
@@ -2132,7 +1980,7 @@
         <v>42</v>
       </c>
       <c r="F27" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>77</v>
       </c>
       <c r="G27" s="4">
@@ -2152,10 +2000,7 @@
       </c>
       <c r="L27" s="2"/>
       <c r="M27" s="2"/>
-      <c r="N27" s="2">
-        <f t="shared" si="1"/>
-        <v>0.23238831512003569</v>
-      </c>
+      <c r="N27" s="2"/>
       <c r="P27" s="2"/>
       <c r="Q27" s="2"/>
       <c r="R27" s="2"/>
@@ -2177,7 +2022,7 @@
         <v>59</v>
       </c>
       <c r="F28" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>108</v>
       </c>
       <c r="G28" s="4">
@@ -2193,10 +2038,7 @@
       </c>
       <c r="L28" s="2"/>
       <c r="M28" s="2"/>
-      <c r="N28" s="2">
-        <f t="shared" si="1"/>
-        <v>0.19548231205456293</v>
-      </c>
+      <c r="N28" s="2"/>
       <c r="P28" s="2"/>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.2">
@@ -2216,7 +2058,7 @@
         <v>24</v>
       </c>
       <c r="F29" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>75</v>
       </c>
       <c r="G29" s="4">
@@ -2237,10 +2079,6 @@
       </c>
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
-      <c r="O29">
-        <f t="shared" si="2"/>
-        <v>0.24757054847171994</v>
-      </c>
       <c r="P29" s="2"/>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.2">
@@ -2260,7 +2098,7 @@
         <v>168</v>
       </c>
       <c r="F30" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>829</v>
       </c>
       <c r="G30" s="4">
@@ -2279,14 +2117,7 @@
         <v>-3.43</v>
       </c>
       <c r="N30" s="2"/>
-      <c r="O30">
-        <f t="shared" si="2"/>
-        <v>8.6414186029710266E-2</v>
-      </c>
-      <c r="P30" s="2">
-        <f t="shared" si="3"/>
-        <v>0.12066929442047349</v>
-      </c>
+      <c r="P30" s="2"/>
     </row>
     <row r="31" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
@@ -2305,7 +2136,7 @@
         <v>61</v>
       </c>
       <c r="F31" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>419</v>
       </c>
       <c r="G31" s="4" t="s">
@@ -2325,18 +2156,9 @@
       <c r="M31" s="2">
         <v>-0.1</v>
       </c>
-      <c r="N31" s="2">
-        <f t="shared" si="1"/>
-        <v>0.13876409404405923</v>
-      </c>
-      <c r="O31">
-        <f t="shared" si="2"/>
-        <v>0.13910465077583697</v>
-      </c>
-      <c r="P31" s="2">
-        <f t="shared" si="3"/>
-        <v>0.13855927210605806</v>
-      </c>
+      <c r="N31" s="2"/>
+      <c r="O31"/>
+      <c r="P31" s="2"/>
       <c r="Q31" s="2"/>
       <c r="R31" s="2"/>
     </row>
@@ -2357,7 +2179,7 @@
         <v>63</v>
       </c>
       <c r="F32" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>150</v>
       </c>
       <c r="G32" s="4">
@@ -2377,10 +2199,7 @@
       </c>
       <c r="L32" s="2"/>
       <c r="M32" s="2"/>
-      <c r="N32" s="2">
-        <f t="shared" si="1"/>
-        <v>0.16553127221136321</v>
-      </c>
+      <c r="N32" s="2"/>
       <c r="O32"/>
       <c r="P32" s="2"/>
       <c r="Q32" s="2"/>
@@ -2422,10 +2241,7 @@
       </c>
       <c r="L33" s="11"/>
       <c r="M33" s="11"/>
-      <c r="N33" s="2">
-        <f t="shared" si="1"/>
-        <v>0.230068352001363</v>
-      </c>
+      <c r="N33" s="2"/>
       <c r="O33"/>
       <c r="P33" s="2"/>
     </row>
@@ -2465,10 +2281,7 @@
       </c>
       <c r="L34" s="11"/>
       <c r="M34" s="11"/>
-      <c r="N34" s="2">
-        <f t="shared" si="1"/>
-        <v>0.22303845514838019</v>
-      </c>
+      <c r="N34" s="2"/>
       <c r="O34"/>
       <c r="P34" s="2"/>
     </row>
@@ -2619,15 +2432,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C4FF05C-65B7-4CF6-8702-24FB92544144}">
-  <dimension ref="A1:J36"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="41.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>41</v>
       </c>
@@ -2652,14 +2468,8 @@
       <c r="H1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -2684,16 +2494,8 @@
       <c r="H2" s="2">
         <v>0.04</v>
       </c>
-      <c r="I2">
-        <f>SQRT((C2+D2)/(C2*D2)+G2^2/(2*(C2+D2)))</f>
-        <v>0.18475372863020592</v>
-      </c>
-      <c r="J2">
-        <f>SQRT((C2+D2)/(C2*D2)+H2^2/(2*(C2+D2)))</f>
-        <v>0.18367602298404209</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -2718,16 +2520,8 @@
       <c r="H3" s="2">
         <v>0.03</v>
       </c>
-      <c r="I3">
-        <f t="shared" ref="I3:I36" si="0">SQRT((C3+D3)/(C3*D3)+G3^2/(2*(C3+D3)))</f>
-        <v>0.18366801638489966</v>
-      </c>
-      <c r="J3">
-        <f t="shared" ref="J3:J36" si="1">SQRT((C3+D3)/(C3*D3)+H3^2/(2*(C3+D3)))</f>
-        <v>0.18366801638489966</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -2752,16 +2546,8 @@
       <c r="H4" s="2">
         <v>-0.21</v>
       </c>
-      <c r="I4">
-        <f t="shared" si="0"/>
-        <v>0.2888933626790342</v>
-      </c>
-      <c r="J4">
-        <f t="shared" si="1"/>
-        <v>0.2894697019263559</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -2786,16 +2572,8 @@
       <c r="H5" s="2">
         <v>-1.26</v>
       </c>
-      <c r="I5">
-        <f t="shared" si="0"/>
-        <v>0.13746026192572441</v>
-      </c>
-      <c r="J5">
-        <f t="shared" si="1"/>
-        <v>0.14616881886602476</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -2820,16 +2598,8 @@
       <c r="H6" s="2">
         <v>1.33</v>
       </c>
-      <c r="I6">
-        <f t="shared" si="0"/>
-        <v>0.19776582301984583</v>
-      </c>
-      <c r="J6">
-        <f t="shared" si="1"/>
-        <v>0.21466186662081385</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -2854,16 +2624,8 @@
       <c r="H7" s="2">
         <v>0.93</v>
       </c>
-      <c r="I7">
-        <f t="shared" si="0"/>
-        <v>0.20364716990746703</v>
-      </c>
-      <c r="J7">
-        <f t="shared" si="1"/>
-        <v>0.20448854744883843</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -2888,16 +2650,8 @@
       <c r="H8" s="2">
         <v>1.52</v>
       </c>
-      <c r="I8">
-        <f t="shared" si="0"/>
-        <v>0.23113307854999898</v>
-      </c>
-      <c r="J8">
-        <f t="shared" si="1"/>
-        <v>0.25385034961567415</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -2922,16 +2676,8 @@
       <c r="H9" s="2">
         <v>0.55000000000000004</v>
       </c>
-      <c r="I9">
-        <f t="shared" si="0"/>
-        <v>0.22891592343041584</v>
-      </c>
-      <c r="J9">
-        <f t="shared" si="1"/>
-        <v>0.22779513822731162</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -2956,16 +2702,8 @@
       <c r="H10" s="2">
         <v>0.38</v>
       </c>
-      <c r="I10">
-        <f t="shared" si="0"/>
-        <v>0.29140231559681423</v>
-      </c>
-      <c r="J10">
-        <f t="shared" si="1"/>
-        <v>0.28881355355810223</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -2988,12 +2726,8 @@
         <v>-0.8</v>
       </c>
       <c r="H11" s="2"/>
-      <c r="I11">
-        <f t="shared" si="0"/>
-        <v>0.23841582427170788</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -3016,12 +2750,8 @@
         <v>-0.86</v>
       </c>
       <c r="H12" s="2"/>
-      <c r="I12">
-        <f t="shared" si="0"/>
-        <v>0.21335123622796281</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -3044,12 +2774,8 @@
       <c r="H13" s="2">
         <v>1.65</v>
       </c>
-      <c r="J13">
-        <f t="shared" si="1"/>
-        <v>0.3661027861134083</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -3074,16 +2800,8 @@
       <c r="H14" s="2">
         <v>0.36</v>
       </c>
-      <c r="I14">
-        <f t="shared" si="0"/>
-        <v>0.17133960242943319</v>
-      </c>
-      <c r="J14">
-        <f t="shared" si="1"/>
-        <v>0.17250661797747513</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -3108,16 +2826,8 @@
       <c r="H15" s="2">
         <v>-0.28999999999999998</v>
       </c>
-      <c r="I15">
-        <f t="shared" si="0"/>
-        <v>0.18969235528922196</v>
-      </c>
-      <c r="J15">
-        <f t="shared" si="1"/>
-        <v>0.18666884748315574</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -3142,16 +2852,8 @@
       <c r="H16" s="2">
         <v>0</v>
       </c>
-      <c r="I16">
-        <f t="shared" si="0"/>
-        <v>0.19280260586305933</v>
-      </c>
-      <c r="J16">
-        <f t="shared" si="1"/>
-        <v>0.18569533817705186</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -3176,16 +2878,8 @@
       <c r="H17" s="2">
         <v>0.33</v>
       </c>
-      <c r="I17">
-        <f t="shared" si="0"/>
-        <v>0.11568464641269635</v>
-      </c>
-      <c r="J17">
-        <f t="shared" si="1"/>
-        <v>0.11620270835411668</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -3210,16 +2904,8 @@
       <c r="H18" s="2">
         <v>-0.7</v>
       </c>
-      <c r="I18">
-        <f t="shared" si="0"/>
-        <v>0.30152830411392256</v>
-      </c>
-      <c r="J18">
-        <f t="shared" si="1"/>
-        <v>0.31060790834631485</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -3244,16 +2930,8 @@
       <c r="H19" s="2">
         <v>-1.06</v>
       </c>
-      <c r="I19">
-        <f t="shared" si="0"/>
-        <v>0.26760511953249322</v>
-      </c>
-      <c r="J19">
-        <f t="shared" si="1"/>
-        <v>0.26697963405473457</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>35</v>
       </c>
@@ -3278,16 +2956,8 @@
       <c r="H20" s="2">
         <v>-0.24</v>
       </c>
-      <c r="I20">
-        <f t="shared" si="0"/>
-        <v>0.25</v>
-      </c>
-      <c r="J20">
-        <f t="shared" si="1"/>
-        <v>0.25089838580588758</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>36</v>
       </c>
@@ -3312,16 +2982,8 @@
       <c r="H21" s="2">
         <v>0.48</v>
       </c>
-      <c r="I21">
-        <f t="shared" si="0"/>
-        <v>0.26760511953249322</v>
-      </c>
-      <c r="J21">
-        <f t="shared" si="1"/>
-        <v>0.25357444666211931</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -3344,12 +3006,8 @@
         <v>0.05</v>
       </c>
       <c r="H22" s="2"/>
-      <c r="I22">
-        <f t="shared" si="0"/>
-        <v>0.24757054847171994</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -3372,12 +3030,8 @@
         <v>-0.3</v>
       </c>
       <c r="H23" s="2"/>
-      <c r="I23">
-        <f t="shared" si="0"/>
-        <v>0.2901149197588202</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -3402,16 +3056,8 @@
       <c r="H24" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="I24">
-        <f t="shared" si="0"/>
-        <v>0.17165286447465111</v>
-      </c>
-      <c r="J24">
-        <f t="shared" si="1"/>
-        <v>0.17155109854432499</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -3436,16 +3082,8 @@
       <c r="H25" s="2">
         <v>0.04</v>
       </c>
-      <c r="I25">
-        <f t="shared" si="0"/>
-        <v>0.17173958569333295</v>
-      </c>
-      <c r="J25">
-        <f t="shared" si="1"/>
-        <v>0.1715157341436159</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -3470,16 +3108,8 @@
       <c r="H26" s="2">
         <v>0.75</v>
       </c>
-      <c r="I26">
-        <f t="shared" si="0"/>
-        <v>0.18259244234085922</v>
-      </c>
-      <c r="J26">
-        <f t="shared" si="1"/>
-        <v>0.18888378261071895</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -3504,16 +3134,8 @@
       <c r="H27" s="2">
         <v>-0.04</v>
       </c>
-      <c r="I27">
-        <f t="shared" si="0"/>
-        <v>0.18264720090929398</v>
-      </c>
-      <c r="J27">
-        <f t="shared" si="1"/>
-        <v>0.18259244234085922</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -3538,16 +3160,8 @@
       <c r="H28" s="2">
         <v>-0.19</v>
       </c>
-      <c r="I28">
-        <f t="shared" si="0"/>
-        <v>0.24117918572405303</v>
-      </c>
-      <c r="J28">
-        <f t="shared" si="1"/>
-        <v>0.23968187171022609</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -3570,12 +3184,8 @@
         <v>-1.1299999999999999</v>
       </c>
       <c r="H29" s="2"/>
-      <c r="I29">
-        <f t="shared" si="0"/>
-        <v>0.20216920487799878</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -3598,12 +3208,8 @@
         <v>-0.89</v>
       </c>
       <c r="H30" s="2"/>
-      <c r="I30">
-        <f t="shared" si="0"/>
-        <v>0.19743008231017442</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -3626,12 +3232,8 @@
       <c r="H31" s="2">
         <v>-1.93</v>
       </c>
-      <c r="J31">
-        <f t="shared" si="1"/>
-        <v>0.2280392653060917</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -3654,12 +3256,8 @@
       <c r="H32" s="2">
         <v>-1.59</v>
       </c>
-      <c r="J32">
-        <f t="shared" si="1"/>
-        <v>0.21701840587506674</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -3684,16 +3282,8 @@
       <c r="H33" s="2">
         <v>-0.1</v>
       </c>
-      <c r="I33">
-        <f t="shared" si="0"/>
-        <v>0.14131409792796853</v>
-      </c>
-      <c r="J33">
-        <f t="shared" si="1"/>
-        <v>0.13855927210605806</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -3718,16 +3308,8 @@
       <c r="H34" s="2">
         <v>0.03</v>
       </c>
-      <c r="I34">
-        <f t="shared" si="0"/>
-        <v>0.25892901349699249</v>
-      </c>
-      <c r="J34">
-        <f t="shared" si="1"/>
-        <v>0.25639839248690693</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -3752,16 +3334,8 @@
       <c r="H35" s="2">
         <v>-0.44</v>
       </c>
-      <c r="I35">
-        <f t="shared" si="0"/>
-        <v>0.26846630416153161</v>
-      </c>
-      <c r="J35">
-        <f t="shared" si="1"/>
-        <v>0.26144627836355216</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -3785,14 +3359,6 @@
       </c>
       <c r="H36" s="2">
         <v>-0.22</v>
-      </c>
-      <c r="I36">
-        <f t="shared" si="0"/>
-        <v>0.24447009019509933</v>
-      </c>
-      <c r="J36">
-        <f t="shared" si="1"/>
-        <v>0.2242821883253327</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating plots + correcting some es
</commit_message>
<xml_diff>
--- a/data/cumulative_ma_data.xlsx
+++ b/data/cumulative_ma_data.xlsx
@@ -8,16 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abagaini/Documents/PROJECTS/Cumul_MA/cumulative/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33950608-D42B-CE45-A322-1367AF0BC4AE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5B232A1-4379-7F4F-BE6F-75E4D2A185A3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17060" activeTab="1" xr2:uid="{D15F3EFF-771D-497D-BAA4-C31EA9079474}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19160" windowHeight="21600" activeTab="2" xr2:uid="{D15F3EFF-771D-497D-BAA4-C31EA9079474}"/>
   </bookViews>
   <sheets>
     <sheet name="Mata_et_al(2011)" sheetId="2" r:id="rId1"/>
     <sheet name="Best_Charness (2015)" sheetId="1" r:id="rId2"/>
-    <sheet name="Seaman_et_al(2021)" sheetId="3" r:id="rId3"/>
-    <sheet name="Sparrow_et_al(2021)" sheetId="4" r:id="rId4"/>
+    <sheet name="Best_Charness (2015)v2" sheetId="5" r:id="rId3"/>
+    <sheet name="Seaman_et_al(2021)" sheetId="3" r:id="rId4"/>
+    <sheet name="Sparrow_et_al(2021)" sheetId="4" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Best_Charness (2015)v2'!$A$1:$H$36</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -28,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="189">
   <si>
     <t>g_pos</t>
   </si>
@@ -502,13 +506,326 @@
   </si>
   <si>
     <t>Sze</t>
+  </si>
+  <si>
+    <t>Mortality</t>
+  </si>
+  <si>
+    <t>Variable</t>
+  </si>
+  <si>
+    <t>Financial</t>
+  </si>
+  <si>
+    <t>Bruine de Bruin et al. (2007)                                                                 63             56        Mortality      Small                -0.03b                                  0.03b</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Bruine de Bruin, Parker, &amp; Fischhoff (2007)                                        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF2F2A2B"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">63             56       Variable       Variable              0.31a                                 0.04a </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Kim, Goldstein, Hasher, &amp; Zacks </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF2F2A2B"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>(1)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Kim et al. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF2F2A2B"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>(1)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Kim et al. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF2F2A2B"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>(2)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Kim et al.  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF2F2A2B"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>(2)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Mather et al. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF2F2A2B"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>(1)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Mather et al. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF2F2A2B"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>(2)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Mather et al. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF2F2A2B"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>(3)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Mather et al.  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF2F2A2B"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>(4)</t>
+    </r>
+  </si>
+  <si>
+    <t>Mayhorn, Fisk, &amp; Whittle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mayhorn et al. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">McKee </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mikels &amp; Reed </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ronnlund, Karlsson, Laggnas, Larsson, &amp; Lindstrom </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF2F2A2B"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>(1)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ronnlund et al. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF2F2A2B"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>(2)</t>
+    </r>
+  </si>
+  <si>
+    <t>Sproten, Diener, Fiebach, &amp; Schwieren</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Thomas &amp; Millar </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF2F2A2B"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>(1)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Thomas &amp; Millar </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF2F2A2B"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>(2)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Thomas &amp; Millar </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF2F2A2B"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>(3)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Thomas &amp; Millar</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF2F2A2B"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>(4)</t>
+    </r>
+  </si>
+  <si>
+    <t>Tymula Glimcher, Levy, &amp; Belmaker</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Watanabe &amp; Shibutani </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF2F2A2B"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>(1)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Watanabe &amp; Shibutani </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF2F2A2B"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>(2)</t>
+    </r>
+  </si>
+  <si>
+    <t>Weller, Levin, &amp; Denburg</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Woodhead </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF2F2A2B"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>(1)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Woodhead </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF2F2A2B"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>(2)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ronnlund et al. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF2F2A2B"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>(3)</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -530,13 +847,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF2F2A2B"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -551,7 +886,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -582,6 +917,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2434,8 +2774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C4FF05C-65B7-4CF6-8702-24FB92544144}">
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:J1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F24" sqref="F24:F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2690,7 +3030,7 @@
       <c r="D10">
         <v>23</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="17" t="s">
         <v>37</v>
       </c>
       <c r="F10" t="s">
@@ -3047,10 +3387,10 @@
       <c r="E24" t="s">
         <v>38</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F24" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="G24" s="2">
+      <c r="G24" s="16">
         <v>-0.12</v>
       </c>
       <c r="H24" s="2">
@@ -3073,7 +3413,7 @@
       <c r="E25" t="s">
         <v>38</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F25" s="17" t="s">
         <v>39</v>
       </c>
       <c r="G25" s="2">
@@ -3099,7 +3439,7 @@
       <c r="E26" t="s">
         <v>38</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F26" s="17" t="s">
         <v>39</v>
       </c>
       <c r="G26" s="2">
@@ -3125,7 +3465,7 @@
       <c r="E27" t="s">
         <v>38</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F27" s="17" t="s">
         <v>39</v>
       </c>
       <c r="G27" s="2">
@@ -3368,6 +3708,933 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7076518B-B90D-9B41-A0BF-410EFE2B4CC8}">
+  <dimension ref="A1:H36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L36" sqref="L36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="10.83203125" style="18"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="18">
+        <v>1988</v>
+      </c>
+      <c r="C2" s="18">
+        <v>24</v>
+      </c>
+      <c r="D2" s="18">
+        <v>24</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2" s="18">
+        <v>0.11</v>
+      </c>
+      <c r="H2" s="18">
+        <v>-0.21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="18">
+        <v>2001</v>
+      </c>
+      <c r="C3" s="18">
+        <v>26</v>
+      </c>
+      <c r="D3" s="18">
+        <v>23</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" s="18">
+        <v>-0.54</v>
+      </c>
+      <c r="H3" s="18">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="B4" s="18">
+        <v>2012</v>
+      </c>
+      <c r="C4" s="18">
+        <v>38</v>
+      </c>
+      <c r="D4" s="18">
+        <v>38</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="F4" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" s="18">
+        <v>-0.8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="B5" s="18">
+        <v>2012</v>
+      </c>
+      <c r="C5" s="18">
+        <v>48</v>
+      </c>
+      <c r="D5" s="18">
+        <v>48</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="18">
+        <v>-0.86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="18" t="s">
+        <v>169</v>
+      </c>
+      <c r="B6" s="18">
+        <v>2012</v>
+      </c>
+      <c r="C6" s="18">
+        <v>20</v>
+      </c>
+      <c r="D6" s="18">
+        <v>20</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="F6" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="H6" s="18">
+        <v>1.65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="B7" s="18">
+        <v>2012</v>
+      </c>
+      <c r="C7" s="18">
+        <v>107</v>
+      </c>
+      <c r="D7" s="18">
+        <v>50</v>
+      </c>
+      <c r="E7" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="F7" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="18">
+        <v>0.06</v>
+      </c>
+      <c r="H7" s="18">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="18" t="s">
+        <v>172</v>
+      </c>
+      <c r="B8" s="18">
+        <v>2002</v>
+      </c>
+      <c r="C8" s="18">
+        <v>58</v>
+      </c>
+      <c r="D8" s="18">
+        <v>58</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="F8" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="G8" s="18">
+        <v>-0.79</v>
+      </c>
+      <c r="H8" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="B9" s="18">
+        <v>2009</v>
+      </c>
+      <c r="C9" s="18">
+        <v>22</v>
+      </c>
+      <c r="D9" s="18">
+        <v>22</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" s="18">
+        <v>-0.03</v>
+      </c>
+      <c r="H9" s="18">
+        <v>-0.7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="18" t="s">
+        <v>176</v>
+      </c>
+      <c r="B10" s="18">
+        <v>2005</v>
+      </c>
+      <c r="C10" s="18">
+        <v>32</v>
+      </c>
+      <c r="D10" s="18">
+        <v>32</v>
+      </c>
+      <c r="E10" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="F10" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="G10" s="18">
+        <v>0</v>
+      </c>
+      <c r="H10" s="18">
+        <v>-0.24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="18" t="s">
+        <v>188</v>
+      </c>
+      <c r="B11" s="18">
+        <v>2005</v>
+      </c>
+      <c r="C11" s="18">
+        <v>32</v>
+      </c>
+      <c r="D11" s="18">
+        <v>32</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="F11" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="G11" s="18">
+        <v>1.08</v>
+      </c>
+      <c r="H11" s="18">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="B12" s="18">
+        <v>2010</v>
+      </c>
+      <c r="C12" s="18">
+        <v>51</v>
+      </c>
+      <c r="D12" s="18">
+        <v>24</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="F12" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="G12" s="18">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="18">
+        <v>2012</v>
+      </c>
+      <c r="C13" s="18">
+        <v>36</v>
+      </c>
+      <c r="D13" s="18">
+        <v>18</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="F13" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="G13" s="18">
+        <v>-0.3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="B14" s="18">
+        <v>2012</v>
+      </c>
+      <c r="C14" s="18">
+        <v>68</v>
+      </c>
+      <c r="D14" s="18">
+        <v>68</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="F14" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="G14" s="18">
+        <v>0.12</v>
+      </c>
+      <c r="H14" s="18">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="B15" s="18">
+        <v>2012</v>
+      </c>
+      <c r="C15" s="18">
+        <v>68</v>
+      </c>
+      <c r="D15" s="18">
+        <v>68</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="G15" s="18">
+        <v>-0.15</v>
+      </c>
+      <c r="H15" s="18">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="B16" s="18">
+        <v>2012</v>
+      </c>
+      <c r="C16" s="18">
+        <v>60</v>
+      </c>
+      <c r="D16" s="18">
+        <v>60</v>
+      </c>
+      <c r="E16" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="F16" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="G16" s="18">
+        <v>-0.04</v>
+      </c>
+      <c r="H16" s="18">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="18" t="s">
+        <v>181</v>
+      </c>
+      <c r="B17" s="18">
+        <v>2012</v>
+      </c>
+      <c r="C17" s="18">
+        <v>60</v>
+      </c>
+      <c r="D17" s="18">
+        <v>60</v>
+      </c>
+      <c r="E17" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="F17" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="G17" s="18">
+        <v>-0.08</v>
+      </c>
+      <c r="H17" s="18">
+        <v>-0.04</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="18" t="s">
+        <v>182</v>
+      </c>
+      <c r="B18" s="18">
+        <v>2012</v>
+      </c>
+      <c r="C18" s="18">
+        <v>34</v>
+      </c>
+      <c r="D18" s="18">
+        <v>36</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="F18" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="G18" s="18">
+        <v>-0.37</v>
+      </c>
+      <c r="H18" s="18">
+        <v>-0.19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="18" t="s">
+        <v>185</v>
+      </c>
+      <c r="B19" s="18">
+        <v>2011</v>
+      </c>
+      <c r="C19" s="18">
+        <v>358</v>
+      </c>
+      <c r="D19" s="18">
+        <v>61</v>
+      </c>
+      <c r="E19" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="F19" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="G19" s="18">
+        <v>-0.81</v>
+      </c>
+      <c r="H19" s="18">
+        <v>-0.1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="B20" s="18">
+        <v>2007</v>
+      </c>
+      <c r="C20" s="18">
+        <v>63</v>
+      </c>
+      <c r="D20" s="18">
+        <v>56</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="F20" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="G20" s="18">
+        <v>-0.03</v>
+      </c>
+      <c r="H20" s="18">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="18">
+        <v>2013</v>
+      </c>
+      <c r="C21" s="18">
+        <v>119</v>
+      </c>
+      <c r="D21" s="18">
+        <v>106</v>
+      </c>
+      <c r="E21" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="F21" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="G21" s="18">
+        <v>-0.69</v>
+      </c>
+      <c r="H21" s="18">
+        <v>-1.26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="B22" s="18">
+        <v>2005</v>
+      </c>
+      <c r="C22" s="18">
+        <v>53</v>
+      </c>
+      <c r="D22" s="18">
+        <v>53</v>
+      </c>
+      <c r="E22" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="F22" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="G22" s="18">
+        <v>0.54</v>
+      </c>
+      <c r="H22" s="18">
+        <v>1.33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="B23" s="18">
+        <v>2005</v>
+      </c>
+      <c r="C23" s="18">
+        <v>53</v>
+      </c>
+      <c r="D23" s="18">
+        <v>53</v>
+      </c>
+      <c r="E23" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="F23" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="G23" s="18">
+        <v>0.89</v>
+      </c>
+      <c r="H23" s="18">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="B24" s="18">
+        <v>2005</v>
+      </c>
+      <c r="C24" s="18">
+        <v>40</v>
+      </c>
+      <c r="D24" s="18">
+        <v>40</v>
+      </c>
+      <c r="E24" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="F24" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="G24" s="18">
+        <v>-0.74</v>
+      </c>
+      <c r="H24" s="18">
+        <v>1.52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="B25" s="18">
+        <v>2005</v>
+      </c>
+      <c r="C25" s="18">
+        <v>40</v>
+      </c>
+      <c r="D25" s="18">
+        <v>40</v>
+      </c>
+      <c r="E25" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="F25" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="G25" s="18">
+        <v>-0.62</v>
+      </c>
+      <c r="H25" s="18">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="B26" s="18">
+        <v>2001</v>
+      </c>
+      <c r="C26" s="18">
+        <v>166</v>
+      </c>
+      <c r="D26" s="18">
+        <v>137</v>
+      </c>
+      <c r="E26" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="F26" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="G26" s="18">
+        <v>0.19</v>
+      </c>
+      <c r="H26" s="18">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="B27" s="18">
+        <v>2005</v>
+      </c>
+      <c r="C27" s="18">
+        <v>32</v>
+      </c>
+      <c r="D27" s="18">
+        <v>32</v>
+      </c>
+      <c r="E27" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="F27" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="G27" s="18">
+        <v>-1.08</v>
+      </c>
+      <c r="H27" s="18">
+        <v>-1.06</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="18" t="s">
+        <v>183</v>
+      </c>
+      <c r="B28" s="18">
+        <v>2010</v>
+      </c>
+      <c r="C28" s="18">
+        <v>41</v>
+      </c>
+      <c r="D28" s="18">
+        <v>87</v>
+      </c>
+      <c r="E28" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="F28" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="G28" s="18">
+        <v>-1.1299999999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="18" t="s">
+        <v>183</v>
+      </c>
+      <c r="B29" s="18">
+        <v>2010</v>
+      </c>
+      <c r="C29" s="18">
+        <v>41</v>
+      </c>
+      <c r="D29" s="18">
+        <v>87</v>
+      </c>
+      <c r="E29" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="F29" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="G29" s="18">
+        <v>-0.89</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="18" t="s">
+        <v>184</v>
+      </c>
+      <c r="B30" s="18">
+        <v>2010</v>
+      </c>
+      <c r="C30" s="18">
+        <v>41</v>
+      </c>
+      <c r="D30" s="18">
+        <v>81</v>
+      </c>
+      <c r="E30" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="F30" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="H30" s="18">
+        <v>-1.93</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="18" t="s">
+        <v>184</v>
+      </c>
+      <c r="B31" s="18">
+        <v>2010</v>
+      </c>
+      <c r="C31" s="18">
+        <v>41</v>
+      </c>
+      <c r="D31" s="18">
+        <v>81</v>
+      </c>
+      <c r="E31" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="F31" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="H31" s="18">
+        <v>-1.59</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="18" t="s">
+        <v>186</v>
+      </c>
+      <c r="B32" s="18">
+        <v>2006</v>
+      </c>
+      <c r="C32" s="18">
+        <v>32</v>
+      </c>
+      <c r="D32" s="18">
+        <v>29</v>
+      </c>
+      <c r="E32" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="F32" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="G32" s="18">
+        <v>-0.4</v>
+      </c>
+      <c r="H32" s="18">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="B33" s="18">
+        <v>2006</v>
+      </c>
+      <c r="C33" s="18">
+        <v>31</v>
+      </c>
+      <c r="D33" s="18">
+        <v>29</v>
+      </c>
+      <c r="E33" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="F33" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="G33" s="18">
+        <v>0.8</v>
+      </c>
+      <c r="H33" s="18">
+        <v>-0.44</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34" s="18">
+        <v>2008</v>
+      </c>
+      <c r="C34" s="18">
+        <v>40</v>
+      </c>
+      <c r="D34" s="18">
+        <v>40</v>
+      </c>
+      <c r="E34" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="F34" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="G34" s="18">
+        <v>-1.25</v>
+      </c>
+      <c r="H34" s="18">
+        <v>-0.22</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="18" t="s">
+        <v>162</v>
+      </c>
+      <c r="B35" s="18">
+        <v>2007</v>
+      </c>
+      <c r="C35" s="18">
+        <v>63</v>
+      </c>
+      <c r="D35" s="18">
+        <v>56</v>
+      </c>
+      <c r="E35" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="F35" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="G35" s="18">
+        <v>0.31</v>
+      </c>
+      <c r="H35" s="18">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="B36" s="18">
+        <v>2002</v>
+      </c>
+      <c r="C36" s="18">
+        <v>58</v>
+      </c>
+      <c r="D36" s="18">
+        <v>58</v>
+      </c>
+      <c r="E36" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="F36" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="G36" s="18">
+        <v>-0.59</v>
+      </c>
+      <c r="H36" s="18">
+        <v>-0.28999999999999998</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0909462-4742-4E90-8AFB-8A146413C5A7}">
   <dimension ref="A1:G45"/>
   <sheetViews>
@@ -4259,7 +5526,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8D7E26E-2B75-4FC8-A793-1D7462D1F2E7}">
   <dimension ref="A1:K17"/>
   <sheetViews>

</xml_diff>